<commit_message>
look at different ways of graphing changes according to different seg measures
</commit_message>
<xml_diff>
--- a/tables/change_in_segs.xlsx
+++ b/tables/change_in_segs.xlsx
@@ -6,16 +6,16 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="accom" r:id="rId3" sheetId="1"/>
-    <sheet name="car" r:id="rId4" sheetId="2"/>
-    <sheet name="cob" r:id="rId5" sheetId="3"/>
-    <sheet name="eth" r:id="rId6" sheetId="4"/>
-    <sheet name="generalhealth" r:id="rId7" sheetId="5"/>
-    <sheet name="llti" r:id="rId8" sheetId="6"/>
-    <sheet name="maritalstatus" r:id="rId9" sheetId="7"/>
-    <sheet name="nssec" r:id="rId10" sheetId="8"/>
-    <sheet name="pensioners" r:id="rId11" sheetId="9"/>
-    <sheet name="religion" r:id="rId12" sheetId="10"/>
+    <sheet name="Grade 1 or 2" r:id="rId3" sheetId="1"/>
+    <sheet name="LLTI" r:id="rId4" sheetId="2"/>
+    <sheet name="No Car" r:id="rId5" sheetId="3"/>
+    <sheet name="Non-house" r:id="rId6" sheetId="4"/>
+    <sheet name="Non-religious" r:id="rId7" sheetId="5"/>
+    <sheet name="Not Scottish" r:id="rId8" sheetId="6"/>
+    <sheet name="Not White" r:id="rId9" sheetId="7"/>
+    <sheet name="Pensioner" r:id="rId10" sheetId="8"/>
+    <sheet name="Poor Health" r:id="rId11" sheetId="9"/>
+    <sheet name="Single" r:id="rId12" sheetId="10"/>
   </sheets>
 </workbook>
 </file>
@@ -226,16 +226,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0031914893617021136</v>
+        <v>-0.05062205062205064</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.01486417221937475</v>
+        <v>-0.031156156156156266</v>
       </c>
       <c r="E2" t="n">
-        <v>0.009522272433828123</v>
+        <v>-0.01414617716402823</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.009795782832475354</v>
+        <v>0.025995948683322025</v>
       </c>
     </row>
     <row r="3">
@@ -246,16 +246,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>0.014116749332315838</v>
+        <v>-0.04161073825503345</v>
       </c>
       <c r="D3" t="n">
-        <v>0.030082987551867217</v>
+        <v>-0.009248554913294743</v>
       </c>
       <c r="E3" t="n">
-        <v>0.022332506203473865</v>
+        <v>0.015408320493066126</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.010692588092344982</v>
+        <v>0.061716006021073785</v>
       </c>
     </row>
     <row r="4">
@@ -266,16 +266,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00750876022025688</v>
+        <v>-0.04771677783478709</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0016207455429498034</v>
+        <v>-0.024021352313167207</v>
       </c>
       <c r="E4" t="n">
-        <v>0.012965363956288212</v>
+        <v>-0.003980891719745226</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.009304128707113833</v>
+        <v>0.040332147093712876</v>
       </c>
     </row>
     <row r="5">
@@ -286,16 +286,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>0.005844258410993582</v>
+        <v>-0.04922515952597996</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.009149130832570913</v>
+        <v>-0.027966440271674123</v>
       </c>
       <c r="E5" t="n">
-        <v>0.010246240290860988</v>
+        <v>-0.012798339674853118</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.009717161200763576</v>
+        <v>0.029287226534933063</v>
       </c>
     </row>
     <row r="6">
@@ -306,16 +306,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>0.013321084060633835</v>
+        <v>-0.10620915032679737</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.06153846153846144</v>
+        <v>-0.07030129124820662</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.012039312039311943</v>
+        <v>-0.025219298245613996</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.03749062734316424</v>
+        <v>0.01795735129068467</v>
       </c>
     </row>
     <row r="7">
@@ -326,16 +326,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>0.003921568627451093</v>
+        <v>-0.057411907654920935</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.023020625415834974</v>
+        <v>-0.032538569424964935</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0052083333333333235</v>
+        <v>-0.010958904109589078</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.014743589743589827</v>
+        <v>0.014790674354474847</v>
       </c>
     </row>
     <row r="8">
@@ -346,16 +346,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.038507821901323645</v>
+        <v>-0.09444444444444446</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.13186813186813198</v>
+        <v>-0.07281553398058259</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.10053619302949052</v>
+        <v>-0.025925925925925897</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.1352564102564103</v>
+        <v>0.03488372093023261</v>
       </c>
     </row>
     <row r="9">
@@ -366,16 +366,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>0.004458161865569162</v>
+        <v>-0.10348837209302317</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.06700610997963337</v>
+        <v>-0.06700507614213207</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.021823562049195343</v>
+        <v>-0.0222222222222222</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.0450584090487669</v>
+        <v>0.027397260273972605</v>
       </c>
     </row>
     <row r="10">
@@ -386,16 +386,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>0.003792667509481672</v>
+        <v>-0.107264086897488</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.04594832648267762</v>
+        <v>-0.06520450503852983</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.007705593197821213</v>
+        <v>-0.019514516896715944</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.028708133971291804</v>
+        <v>0.020216267042783256</v>
       </c>
     </row>
     <row r="11">
@@ -406,16 +406,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0.020806451612903263</v>
+        <v>-0.003205128205128233</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.029113509977101795</v>
+        <v>-0.030062111801242235</v>
       </c>
       <c r="E11" t="n">
-        <v>0.033467974610502015</v>
+        <v>-0.03102153724560362</v>
       </c>
       <c r="F11" t="n">
-        <v>0.012632496006969713</v>
+        <v>-0.06037567084078705</v>
       </c>
     </row>
     <row r="12">
@@ -426,16 +426,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>0.020162128455622503</v>
+        <v>-0.10619469026548678</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.04808877928483358</v>
+        <v>-0.07525655644241727</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0019153011278995784</v>
+        <v>-0.03015075376884427</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.02510368915084045</v>
+        <v>-0.0034904013961605377</v>
       </c>
     </row>
     <row r="13">
@@ -446,16 +446,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.0035846072746441313</v>
+        <v>-0.038313685289595126</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.01270662318677609</v>
+        <v>-0.04792746113989641</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.007689698066267136</v>
+        <v>-0.019701419481155166</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.009146739840585399</v>
+        <v>-0.028834894613583212</v>
       </c>
     </row>
     <row r="14">
@@ -466,16 +466,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>0.006069485140226065</v>
+        <v>-0.04044585987261143</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.0011800042909246833</v>
+        <v>-0.03336791147994465</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.025873362445414907</v>
+        <v>-0.020723504817306084</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0072940332416596846</v>
+        <v>0.02327746741154554</v>
       </c>
     </row>
     <row r="15">
@@ -486,16 +486,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.060171256653552475</v>
+        <v>0.1138952164009111</v>
       </c>
       <c r="D15" t="n">
-        <v>0.042244835029294006</v>
+        <v>0.18924581005586602</v>
       </c>
       <c r="E15" t="n">
-        <v>0.14637514384349826</v>
+        <v>0.03293687099725532</v>
       </c>
       <c r="F15" t="n">
-        <v>0.09820298658567451</v>
+        <v>-0.07419505366308912</v>
       </c>
     </row>
     <row r="16">
@@ -506,16 +506,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.040076313263577065</v>
+        <v>0.05941500087673148</v>
       </c>
       <c r="D16" t="n">
-        <v>0.028759493670886056</v>
+        <v>0.020290166997661816</v>
       </c>
       <c r="E16" t="n">
-        <v>0.006846403740474328</v>
+        <v>0.028734211122787328</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.019219685213921624</v>
+        <v>-0.022714879694635707</v>
       </c>
     </row>
     <row r="17">
@@ -526,16 +526,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>0.009554140127388514</v>
+        <v>-0.12589928057553956</v>
       </c>
       <c r="D17" t="n">
-        <v>0.015401540154015386</v>
+        <v>-0.07692307692307705</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.03993344425956738</v>
+        <v>-0.052924791086350946</v>
       </c>
       <c r="F17" t="n">
-        <v>0.015624999999999905</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
@@ -546,16 +546,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>0.03939514524472727</v>
+        <v>-0.015067805123053755</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.022899159663865475</v>
+        <v>-0.04591688462656215</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0463900134952766</v>
+        <v>-0.04006063230835851</v>
       </c>
       <c r="F18" t="n">
-        <v>0.037805521364515496</v>
+        <v>-0.06663196251952111</v>
       </c>
     </row>
     <row r="19">
@@ -566,16 +566,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2</v>
+        <v>-0.2000000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>0.31617647058823534</v>
+        <v>-0.06451612903225809</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0</v>
+        <v>-0.18750000000000008</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9374999999999999</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="20">
@@ -586,16 +586,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0056848653866780775</v>
+        <v>-0.025724683147195473</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.022071307300509265</v>
+        <v>-0.03677793324005591</v>
       </c>
       <c r="E20" t="n">
-        <v>-1.1268875366237208E-4</v>
+        <v>-0.010642341315089272</v>
       </c>
       <c r="F20" t="n">
-        <v>0.011982248520710052</v>
+        <v>0.04120824164832957</v>
       </c>
     </row>
   </sheetData>
@@ -637,16 +637,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.2439189189189189</v>
+        <v>-0.018244013683010363</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1793760831889081</v>
+        <v>0.10619803476946339</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.10170870626525629</v>
+        <v>-0.013269819666553299</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0073637702503681944</v>
+        <v>0.03562054743157109</v>
       </c>
     </row>
     <row r="3">
@@ -657,16 +657,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.39793814432989694</v>
+        <v>-0.008324084350721428</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1637239165329052</v>
+        <v>0.20423892100192675</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.21109607577807846</v>
+        <v>-0.004162330905307091</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.0816542948038176</v>
+        <v>0.051546391752577365</v>
       </c>
     </row>
     <row r="4">
@@ -677,16 +677,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.29976019184652275</v>
+        <v>-0.011116051578479334</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1789242590559824</v>
+        <v>0.14126394052044614</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.14042126379137412</v>
+        <v>-0.01010101010101011</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.02403433476394859</v>
+        <v>0.04216600088770532</v>
       </c>
     </row>
     <row r="5">
@@ -697,16 +697,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.2609006433166547</v>
+        <v>-0.013682092555331937</v>
       </c>
       <c r="D5" t="n">
-        <v>0.17580340264650274</v>
+        <v>0.1194274028629857</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.10792580101180432</v>
+        <v>-0.012955182072829259</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.0015420200462606453</v>
+        <v>0.03773584905660376</v>
       </c>
     </row>
     <row r="6">
@@ -717,16 +717,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.3644444444444444</v>
+        <v>-0.06532663316582928</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5037037037037037</v>
+        <v>0.17408376963350794</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.17610062893081763</v>
+        <v>-0.07011866235167212</v>
       </c>
       <c r="F6" t="n">
-        <v>0.058823529411764684</v>
+        <v>0.05412719891745608</v>
       </c>
     </row>
     <row r="7">
@@ -737,16 +737,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.21648460774577954</v>
+        <v>-0.025568980050575996</v>
       </c>
       <c r="D7" t="n">
-        <v>0.19148936170212777</v>
+        <v>0.08936525612472149</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1007615700058582</v>
+        <v>-0.021415973796926058</v>
       </c>
       <c r="F7" t="n">
-        <v>0.009292720702116654</v>
+        <v>0.0329183955739973</v>
       </c>
     </row>
     <row r="8">
@@ -757,16 +757,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.36507936507936506</v>
+        <v>-0.05714285714285713</v>
       </c>
       <c r="D8" t="n">
-        <v>0.44999999999999984</v>
+        <v>0.18750000000000006</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.17777777777777767</v>
+        <v>-0.05098039215686271</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01639344262295072</v>
+        <v>0.0724637681159421</v>
       </c>
     </row>
     <row r="9">
@@ -777,16 +777,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.3682539682539682</v>
+        <v>-0.05887681159420283</v>
       </c>
       <c r="D9" t="n">
-        <v>0.44162436548223366</v>
+        <v>0.19007490636704105</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.19026548672566365</v>
+        <v>-0.06346749226006201</v>
       </c>
       <c r="F9" t="n">
-        <v>0.009740259740259681</v>
+        <v>0.06445312499999994</v>
       </c>
     </row>
     <row r="10">
@@ -797,16 +797,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.36684303350970016</v>
+        <v>-0.06032818532818525</v>
       </c>
       <c r="D10" t="n">
-        <v>0.43589743589743596</v>
+        <v>0.18089944416371906</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.19354838709677422</v>
+        <v>-0.0752458315519453</v>
       </c>
       <c r="F10" t="n">
-        <v>0.008992805755395692</v>
+        <v>0.05530973451327439</v>
       </c>
     </row>
     <row r="11">
@@ -817,16 +817,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1652626362735381</v>
+        <v>0.05404404960207293</v>
       </c>
       <c r="D11" t="n">
-        <v>0.40766666666666673</v>
+        <v>0.09895470383275275</v>
       </c>
       <c r="E11" t="n">
-        <v>0.24157764995891537</v>
+        <v>0.05434782608695648</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3283828382838284</v>
+        <v>0.08183800100620485</v>
       </c>
     </row>
     <row r="12">
@@ -837,16 +837,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.34448160535117056</v>
+        <v>-0.07258834765998086</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6728395061728395</v>
+        <v>0.1384152457372117</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.1310679611650486</v>
+        <v>-0.07749999999999992</v>
       </c>
       <c r="F12" t="n">
-        <v>0.19196428571428578</v>
+        <v>0.030769230769230795</v>
       </c>
     </row>
     <row r="13">
@@ -857,16 +857,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.043707796193983996</v>
+        <v>-0.022936327798351447</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.03238916256157648</v>
+        <v>-0.017948096046568076</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.02096793855906375</v>
+        <v>-0.010233566096797438</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.014035087719298322</v>
+        <v>-0.008780768677126809</v>
       </c>
     </row>
     <row r="14">
@@ -877,16 +877,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.14308847342852946</v>
+        <v>-0.04729945669542996</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.13410067951740398</v>
+        <v>5.042864346948511E-4</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.14885100074128974</v>
+        <v>-0.0368997472620051</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.08119601328903646</v>
+        <v>-0.04019746121297609</v>
       </c>
     </row>
     <row r="15">
@@ -897,16 +897,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.42857142857142855</v>
+        <v>0.10671191553544492</v>
       </c>
       <c r="D15" t="n">
-        <v>1.2848751835535976</v>
+        <v>0.39526484751203855</v>
       </c>
       <c r="E15" t="n">
-        <v>0.7906976744186045</v>
+        <v>0.21423562412342212</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6989079563182525</v>
+        <v>0.31622581918673487</v>
       </c>
     </row>
     <row r="16">
@@ -917,16 +917,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.08952128443069678</v>
+        <v>0.04205636229387166</v>
       </c>
       <c r="D16" t="n">
-        <v>0.011766071912373808</v>
+        <v>3.9455303539231176E-4</v>
       </c>
       <c r="E16" t="n">
-        <v>0.02028682068117373</v>
+        <v>0.013253159896919893</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.014191855109241768</v>
+        <v>-0.0032596305124025456</v>
       </c>
     </row>
     <row r="17">
@@ -937,16 +937,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.15217391304347822</v>
+        <v>-0.07441860465116266</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>0.013245033112582702</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.03246753246753249</v>
+        <v>-0.030612244897959176</v>
       </c>
       <c r="F17" t="n">
-        <v>0.00628930817610059</v>
+        <v>0.005649717514124259</v>
       </c>
     </row>
     <row r="18">
@@ -957,16 +957,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1527254458678723</v>
+        <v>0.04965883244882487</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3862938970337539</v>
+        <v>0.09269863994273456</v>
       </c>
       <c r="E18" t="n">
-        <v>0.23596442468037793</v>
+        <v>0.052303429165223424</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3227603943420488</v>
+        <v>0.07883888698041899</v>
       </c>
     </row>
     <row r="19">
@@ -977,16 +977,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2</v>
+        <v>-0.2000000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3661971830985915</v>
+        <v>0.1260504201680672</v>
       </c>
       <c r="E19" t="n">
-        <v>0.16666666666666677</v>
+        <v>0.22222222222222232</v>
       </c>
       <c r="F19" t="n">
-        <v>1.2727272727272727</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="20">
@@ -997,16 +997,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.031602155805977514</v>
+        <v>-0.012001454721784483</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.021288949100058078</v>
+        <v>-0.002022585538513551</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.008671257332313222</v>
+        <v>-0.004055548728032407</v>
       </c>
       <c r="F20" t="n">
-        <v>0.02426242236024836</v>
+        <v>0.004809343868086419</v>
       </c>
     </row>
   </sheetData>
@@ -1048,16 +1048,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02087332053742799</v>
+        <v>-0.12386706948640488</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.022929936305732503</v>
+        <v>-0.09311740890688261</v>
       </c>
       <c r="E2" t="n">
-        <v>0.013556388808768336</v>
+        <v>-0.11168032786885253</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.06412175648702595</v>
+        <v>-0.11807120324470471</v>
       </c>
     </row>
     <row r="3">
@@ -1068,16 +1068,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>0.06816030293467973</v>
+        <v>-0.1378839590443686</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0485232067510549</v>
+        <v>-0.05607476635514011</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08266414737836555</v>
+        <v>-0.10044642857142856</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.04821638573108587</v>
+        <v>-0.11163416274377945</v>
       </c>
     </row>
     <row r="4">
@@ -1088,16 +1088,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>0.04176771759633526</v>
+        <v>-0.12794033275960995</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0015455950540958282</v>
+        <v>-0.08327501749475154</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03672612801678912</v>
+        <v>-0.11190903650508674</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.059173357121617524</v>
+        <v>-0.11695906432748535</v>
       </c>
     </row>
     <row r="5">
@@ -1108,16 +1108,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>0.028028028028027997</v>
+        <v>-0.1229551451187336</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.01590348231423095</v>
+        <v>-0.08785046728971964</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01668653158522048</v>
+        <v>-0.11152025249868489</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.06338397066526978</v>
+        <v>-0.11856400566839873</v>
       </c>
     </row>
     <row r="6">
@@ -1128,16 +1128,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.01378070701018572</v>
+        <v>-0.24791086350974934</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.06324110671936757</v>
+        <v>-0.1409395973154362</v>
       </c>
       <c r="E6" t="n">
-        <v>0.010928961748633977</v>
+        <v>-0.17971014492753634</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.14440639269406386</v>
+        <v>-0.22601279317697226</v>
       </c>
     </row>
     <row r="7">
@@ -1148,16 +1148,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00509554140127393</v>
+        <v>-0.120923415170392</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.02058590657165472</v>
+        <v>-0.07603305785123968</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0071820870299958055</v>
+        <v>-0.0945945945945947</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.06416217221498972</v>
+        <v>-0.11331351172778327</v>
       </c>
     </row>
     <row r="8">
@@ -1168,16 +1168,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.005050505050505078</v>
+        <v>-0.2540983606557377</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0675675675675675</v>
+        <v>-0.11578947368421055</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.009592326139088671</v>
+        <v>-0.17391304347826086</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.16859504132231407</v>
+        <v>-0.2251655629139073</v>
       </c>
     </row>
     <row r="9">
@@ -1188,16 +1188,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0032258064516128837</v>
+        <v>-0.24190800681431013</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.05346350534635058</v>
+        <v>-0.12147505422993493</v>
       </c>
       <c r="E9" t="n">
-        <v>0.005485463521667586</v>
+        <v>-0.16967509025270755</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.13836734693877545</v>
+        <v>-0.2169680111265647</v>
       </c>
     </row>
     <row r="10">
@@ -1208,16 +1208,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0031914893617020716</v>
+        <v>-0.23205506391347094</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.03899721448467967</v>
+        <v>-0.13135068153655513</v>
       </c>
       <c r="E10" t="n">
-        <v>0.015576323987538955</v>
+        <v>-0.1671891327063741</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.11524774158226123</v>
+        <v>-0.20734693877551014</v>
       </c>
     </row>
     <row r="11">
@@ -1228,16 +1228,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0818595250126326</v>
+        <v>-0.08017334777898148</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.06432160804020096</v>
+        <v>-0.057191634656423365</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0032644178454842247</v>
+        <v>-0.060800790904597155</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0788203753351207</v>
+        <v>-0.0910458991723099</v>
       </c>
     </row>
     <row r="12">
@@ -1248,16 +1248,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.05613648871766641</v>
+        <v>-0.2712933753943218</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.0762112139357649</v>
+        <v>-0.17589576547231275</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01731879409878114</v>
+        <v>-0.20312500000000006</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.14517625231910955</v>
+        <v>-0.2505050505050505</v>
       </c>
     </row>
     <row r="13">
@@ -1268,16 +1268,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>3.2615786040452057E-4</v>
+        <v>-0.03513022410660209</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.006402927052366852</v>
+        <v>-0.019123020706455465</v>
       </c>
       <c r="E13" t="n">
-        <v>9.2571164082391E-4</v>
+        <v>-0.01403808593750008</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.006843800322061183</v>
+        <v>-0.011384925781812808</v>
       </c>
     </row>
     <row r="14">
@@ -1288,16 +1288,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>0.03306981405188726</v>
+        <v>-0.015508395522388033</v>
       </c>
       <c r="D14" t="n">
-        <v>0.012870298457783263</v>
+        <v>0.020378632581695304</v>
       </c>
       <c r="E14" t="n">
-        <v>0.011941669537260264</v>
+        <v>-0.0017736786094360373</v>
       </c>
       <c r="F14" t="n">
-        <v>0.03525681674064686</v>
+        <v>0.032736177342441004</v>
       </c>
     </row>
     <row r="15">
@@ -1308,16 +1308,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.07627475769068691</v>
+        <v>-0.188715953307393</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.007805724197744996</v>
+        <v>-0.10402684563758384</v>
       </c>
       <c r="E15" t="n">
-        <v>0.17987360233349542</v>
+        <v>0.019438444924406006</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.033112582781456984</v>
+        <v>-0.13351498637602183</v>
       </c>
     </row>
     <row r="16">
@@ -1328,16 +1328,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.04716906469126423</v>
+        <v>0.07682308232704019</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.02479854727045745</v>
+        <v>0.030466301953524833</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.05381225797836825</v>
+        <v>0.022615272949535734</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.011869074354466611</v>
+        <v>0.018483885610531072</v>
       </c>
     </row>
     <row r="17">
@@ -1348,16 +1348,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>0.041297935103244796</v>
+        <v>-0.182089552238806</v>
       </c>
       <c r="D17" t="n">
-        <v>0.040522875816993535</v>
+        <v>-0.06989247311827958</v>
       </c>
       <c r="E17" t="n">
-        <v>0.11455847255369925</v>
+        <v>-0.03952569169960478</v>
       </c>
       <c r="F17" t="n">
-        <v>0.043902439024390144</v>
+        <v>-0.044303797468354486</v>
       </c>
     </row>
     <row r="18">
@@ -1368,16 +1368,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.06781166716020129</v>
+        <v>-0.056547619047619097</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.052389705882352915</v>
+        <v>-0.03595812471552125</v>
       </c>
       <c r="E18" t="n">
-        <v>0.028726708074534157</v>
+        <v>-0.03638368246968023</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.06592039800995024</v>
+        <v>-0.06636060100166943</v>
       </c>
     </row>
     <row r="19">
@@ -1388,16 +1388,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.09803921568627459</v>
+        <v>-0.41379310344827586</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6842105263157896</v>
+        <v>-0.2000000000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2173913043478261</v>
+        <v>-0.11111111111111105</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8947368421052632</v>
+        <v>-0.2222222222222222</v>
       </c>
     </row>
     <row r="20">
@@ -1408,16 +1408,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>0.011221802358868695</v>
+        <v>-0.02832574607991904</v>
       </c>
       <c r="D20" t="n">
-        <v>0.020729426433915354</v>
+        <v>-0.0482013113592061</v>
       </c>
       <c r="E20" t="n">
-        <v>0.01705426356589145</v>
+        <v>-0.010800842992623795</v>
       </c>
       <c r="F20" t="n">
-        <v>0.01093329107906832</v>
+        <v>-0.025187566988210078</v>
       </c>
     </row>
   </sheetData>
@@ -1459,16 +1459,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>0.02087332053742799</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>-0.022929936305732503</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0</v>
+        <v>0.013556388808768336</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0</v>
+        <v>-0.06412175648702595</v>
       </c>
     </row>
     <row r="3">
@@ -1479,16 +1479,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>0.06816030293467973</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
+        <v>0.0485232067510549</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0</v>
+        <v>0.08266414737836555</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0</v>
+        <v>-0.04821638573108587</v>
       </c>
     </row>
     <row r="4">
@@ -1499,16 +1499,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0</v>
+        <v>0.04176771759633526</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0</v>
+        <v>-0.0015455950540958282</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0</v>
+        <v>0.03672612801678912</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0</v>
+        <v>-0.059173357121617524</v>
       </c>
     </row>
     <row r="5">
@@ -1519,16 +1519,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>0.028028028028027997</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
+        <v>-0.01590348231423095</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0</v>
+        <v>0.01668653158522048</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0</v>
+        <v>-0.06338397066526978</v>
       </c>
     </row>
     <row r="6">
@@ -1539,16 +1539,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>-0.01378070701018572</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0</v>
+        <v>-0.06324110671936757</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0</v>
+        <v>0.010928961748633977</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0</v>
+        <v>-0.14440639269406386</v>
       </c>
     </row>
     <row r="7">
@@ -1559,16 +1559,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>0.00509554140127393</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
+        <v>-0.02058590657165472</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0</v>
+        <v>0.0071820870299958055</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0</v>
+        <v>-0.06416217221498972</v>
       </c>
     </row>
     <row r="8">
@@ -1579,16 +1579,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0</v>
+        <v>-0.005050505050505078</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0</v>
+        <v>-0.0675675675675675</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0</v>
+        <v>-0.009592326139088671</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0</v>
+        <v>-0.16859504132231407</v>
       </c>
     </row>
     <row r="9">
@@ -1599,16 +1599,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0</v>
+        <v>0.0032258064516128837</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0</v>
+        <v>-0.05346350534635058</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0</v>
+        <v>0.005485463521667586</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0</v>
+        <v>-0.13836734693877545</v>
       </c>
     </row>
     <row r="10">
@@ -1619,16 +1619,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0</v>
+        <v>0.0031914893617020716</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0</v>
+        <v>-0.03899721448467967</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0</v>
+        <v>0.015576323987538955</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0</v>
+        <v>-0.11524774158226123</v>
       </c>
     </row>
     <row r="11">
@@ -1639,16 +1639,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0</v>
+        <v>-0.0818595250126326</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0</v>
+        <v>-0.06432160804020096</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0</v>
+        <v>0.0032644178454842247</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0</v>
+        <v>-0.0788203753351207</v>
       </c>
     </row>
     <row r="12">
@@ -1659,16 +1659,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0</v>
+        <v>-0.05613648871766641</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0</v>
+        <v>-0.0762112139357649</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0</v>
+        <v>0.01731879409878114</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0</v>
+        <v>-0.14517625231910955</v>
       </c>
     </row>
     <row r="13">
@@ -1679,16 +1679,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0</v>
+        <v>3.2615786040452057E-4</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0</v>
+        <v>-0.006402927052366852</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0</v>
+        <v>9.2571164082391E-4</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0</v>
+        <v>-0.006843800322061183</v>
       </c>
     </row>
     <row r="14">
@@ -1699,16 +1699,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0</v>
+        <v>0.03306981405188726</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0</v>
+        <v>0.012870298457783263</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0</v>
+        <v>0.011941669537260264</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0</v>
+        <v>0.03525681674064686</v>
       </c>
     </row>
     <row r="15">
@@ -1719,16 +1719,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0</v>
+        <v>-0.07627475769068691</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0</v>
+        <v>-0.007805724197744996</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0</v>
+        <v>0.17987360233349542</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0</v>
+        <v>-0.033112582781456984</v>
       </c>
     </row>
     <row r="16">
@@ -1739,16 +1739,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0</v>
+        <v>-0.04716906469126423</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0</v>
+        <v>-0.02479854727045745</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0</v>
+        <v>-0.05381225797836825</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0</v>
+        <v>-0.011869074354466611</v>
       </c>
     </row>
     <row r="17">
@@ -1759,16 +1759,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0</v>
+        <v>0.041297935103244796</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>0.040522875816993535</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0</v>
+        <v>0.11455847255369925</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0</v>
+        <v>0.043902439024390144</v>
       </c>
     </row>
     <row r="18">
@@ -1779,16 +1779,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0</v>
+        <v>-0.06781166716020129</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0</v>
+        <v>-0.052389705882352915</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0</v>
+        <v>0.028726708074534157</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0</v>
+        <v>-0.06592039800995024</v>
       </c>
     </row>
     <row r="19">
@@ -1799,16 +1799,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0</v>
+        <v>-0.09803921568627459</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0</v>
+        <v>0.6842105263157896</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0</v>
+        <v>0.2173913043478261</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0</v>
+        <v>0.8947368421052632</v>
       </c>
     </row>
     <row r="20">
@@ -1819,16 +1819,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0</v>
+        <v>0.011221802358868695</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0</v>
+        <v>0.020729426433915354</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0</v>
+        <v>0.01705426356589145</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0</v>
+        <v>0.01093329107906832</v>
       </c>
     </row>
   </sheetData>
@@ -1870,16 +1870,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.020481310803891466</v>
+        <v>0.0031914893617021136</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>-0.01486417221937475</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.055804823331463756</v>
+        <v>0.009522272433828123</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.13854835571122795</v>
+        <v>-0.009795782832475354</v>
       </c>
     </row>
     <row r="3">
@@ -1890,16 +1890,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0473026840287006</v>
+        <v>0.014116749332315838</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.009154929577464823</v>
+        <v>0.030082987551867217</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.09450679267572365</v>
+        <v>0.022332506203473865</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.17800081933633763</v>
+        <v>-0.010692588092344982</v>
       </c>
     </row>
     <row r="4">
@@ -1910,16 +1910,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.033315981259760485</v>
+        <v>0.00750876022025688</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.004124656278643501</v>
+        <v>0.0016207455429498034</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.07292563881711163</v>
+        <v>0.012965363956288212</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.1560509554140127</v>
+        <v>-0.009304128707113833</v>
       </c>
     </row>
     <row r="5">
@@ -1930,16 +1930,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.026532715095311632</v>
+        <v>0.005844258410993582</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0015865820489573401</v>
+        <v>-0.009149130832570913</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.05915492957746469</v>
+        <v>0.010246240290860988</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.144481474220741</v>
+        <v>-0.009717161200763576</v>
       </c>
     </row>
     <row r="6">
@@ -1950,16 +1950,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0418794688457609</v>
+        <v>0.013321084060633835</v>
       </c>
       <c r="D6" t="n">
-        <v>0.021126760563380344</v>
+        <v>-0.06153846153846144</v>
       </c>
       <c r="E6" t="n">
-        <v>0.061757719714964326</v>
+        <v>-0.012039312039311943</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.16817532158170556</v>
+        <v>-0.03749062734316424</v>
       </c>
     </row>
     <row r="7">
@@ -1970,16 +1970,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.036931277365315006</v>
+        <v>0.003921568627451093</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.02466598150051382</v>
+        <v>-0.023020625415834974</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.04113858300436315</v>
+        <v>-0.0052083333333333235</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.1161242603550296</v>
+        <v>-0.014743589743589827</v>
       </c>
     </row>
     <row r="8">
@@ -1990,16 +1990,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.36531365313653136</v>
+        <v>-0.038507821901323645</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.3176206509539843</v>
+        <v>-0.13186813186813198</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.27009646302250795</v>
+        <v>-0.10053619302949052</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.41935483870967744</v>
+        <v>-0.1352564102564103</v>
       </c>
     </row>
     <row r="9">
@@ -2010,16 +2010,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.1219715956558062</v>
+        <v>0.004458161865569162</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.08207646439845678</v>
+        <v>-0.06700610997963337</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.10114030738720874</v>
+        <v>-0.021823562049195343</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.2415902140672784</v>
+        <v>-0.0450584090487669</v>
       </c>
     </row>
     <row r="10">
@@ -2030,16 +2030,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.11000552791597568</v>
+        <v>0.003792667509481672</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.05729653882132827</v>
+        <v>-0.04594832648267762</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.07088186356073206</v>
+        <v>-0.007705593197821213</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.19503063308373048</v>
+        <v>-0.028708133971291804</v>
       </c>
     </row>
     <row r="11">
@@ -2050,16 +2050,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0831556503198294</v>
+        <v>0.020806451612903263</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4781976744186046</v>
+        <v>-0.029113509977101795</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9026548672566371</v>
+        <v>0.033467974610502015</v>
       </c>
       <c r="F11" t="n">
-        <v>0.267524115755627</v>
+        <v>0.012632496006969713</v>
       </c>
     </row>
     <row r="12">
@@ -2070,16 +2070,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7201492537313433</v>
+        <v>0.020162128455622503</v>
       </c>
       <c r="D12" t="n">
-        <v>0.38262910798122074</v>
+        <v>-0.04808877928483358</v>
       </c>
       <c r="E12" t="n">
-        <v>0.7764705882352942</v>
+        <v>0.0019153011278995784</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0651465798045602</v>
+        <v>-0.02510368915084045</v>
       </c>
     </row>
     <row r="13">
@@ -2090,16 +2090,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0015628488501897263</v>
+        <v>-0.0035846072746441313</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.025214966302579654</v>
+        <v>-0.01270662318677609</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.011958146487294556</v>
+        <v>-0.007689698066267136</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.047625144027653325</v>
+        <v>-0.009146739840585399</v>
       </c>
     </row>
     <row r="14">
@@ -2110,16 +2110,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.010397553516819558</v>
+        <v>0.006069485140226065</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.007262684124386247</v>
+        <v>-0.0011800042909246833</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.01412171086050992</v>
+        <v>-0.025873362445414907</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.030967078189300428</v>
+        <v>-0.0072940332416596846</v>
       </c>
     </row>
     <row r="15">
@@ -2130,16 +2130,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>1.5679611650485439</v>
+        <v>0.060171256653552475</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8813056379821957</v>
+        <v>0.042244835029294006</v>
       </c>
       <c r="E15" t="n">
-        <v>1.225941422594142</v>
+        <v>0.14637514384349826</v>
       </c>
       <c r="F15" t="n">
-        <v>0.20491803278688514</v>
+        <v>0.09820298658567451</v>
       </c>
     </row>
     <row r="16">
@@ -2150,16 +2150,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.1060418351779992</v>
+        <v>-0.040076313263577065</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.031006067191886227</v>
+        <v>0.028759493670886056</v>
       </c>
       <c r="E16" t="n">
-        <v>0.008581825207702731</v>
+        <v>0.006846403740474328</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.004736736468856521</v>
+        <v>-0.019219685213921624</v>
       </c>
     </row>
     <row r="17">
@@ -2170,16 +2170,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>0.15863141524105756</v>
+        <v>0.009554140127388514</v>
       </c>
       <c r="D17" t="n">
-        <v>0.100767754318618</v>
+        <v>0.015401540154015386</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.04718693284936488</v>
+        <v>-0.03993344425956738</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.23408624229979466</v>
+        <v>0.015624999999999905</v>
       </c>
     </row>
     <row r="18">
@@ -2190,16 +2190,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>1.7040816326530615</v>
+        <v>0.03939514524472727</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7046004842615011</v>
+        <v>-0.022899159663865475</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9203747072599532</v>
+        <v>0.0463900134952766</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5635018495684339</v>
+        <v>0.037805521364515496</v>
       </c>
     </row>
     <row r="19">
@@ -2210,16 +2210,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2884615384615384</v>
+        <v>-0.2</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9931506849315069</v>
+        <v>0.31617647058823534</v>
       </c>
       <c r="E19" t="n">
         <v>0.0</v>
       </c>
       <c r="F19" t="n">
-        <v>2.666666666666667</v>
+        <v>0.9374999999999999</v>
       </c>
     </row>
     <row r="20">
@@ -2230,16 +2230,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>0.012467476149176013</v>
+        <v>0.0056848653866780775</v>
       </c>
       <c r="D20" t="n">
-        <v>0.010906862745098063</v>
+        <v>-0.022071307300509265</v>
       </c>
       <c r="E20" t="n">
-        <v>6.694934166481198E-4</v>
+        <v>-1.1268875366237208E-4</v>
       </c>
       <c r="F20" t="n">
-        <v>0.011914217633042108</v>
+        <v>0.011982248520710052</v>
       </c>
     </row>
   </sheetData>
@@ -2281,16 +2281,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1660839160839161</v>
+        <v>-0.2439189189189189</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.07484076433121019</v>
+        <v>0.1793760831889081</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.10225140712945598</v>
+        <v>-0.10170870626525629</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.08454312553373179</v>
+        <v>0.0073637702503681944</v>
       </c>
     </row>
     <row r="3">
@@ -2301,16 +2301,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.26457399103139007</v>
+        <v>-0.39793814432989694</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.19405940594059404</v>
+        <v>0.1637239165329052</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.20720221606648195</v>
+        <v>-0.21109607577807846</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.19778481012658217</v>
+        <v>-0.0816542948038176</v>
       </c>
     </row>
     <row r="4">
@@ -2321,16 +2321,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.20612813370473534</v>
+        <v>-0.29976019184652275</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.12339930151338764</v>
+        <v>0.1789242590559824</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.14883955600403634</v>
+        <v>-0.14042126379137412</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.13102480112306972</v>
+        <v>-0.02403433476394859</v>
       </c>
     </row>
     <row r="5">
@@ -2341,16 +2341,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1788109074653554</v>
+        <v>-0.2609006433166547</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.09306167400881056</v>
+        <v>0.17580340264650274</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.11021377672209026</v>
+        <v>-0.10792580101180432</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.09784993418165856</v>
+        <v>-0.0015420200462606453</v>
       </c>
     </row>
     <row r="6">
@@ -2361,16 +2361,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.21282051282051279</v>
+        <v>-0.3644444444444444</v>
       </c>
       <c r="D6" t="n">
-        <v>0.003472222222222201</v>
+        <v>0.5037037037037037</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.08115942028985518</v>
+        <v>-0.17610062893081763</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.08639308855291584</v>
+        <v>0.058823529411764684</v>
       </c>
     </row>
     <row r="7">
@@ -2381,16 +2381,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.15319426336375502</v>
+        <v>-0.21648460774577954</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.05499612703330748</v>
+        <v>0.19148936170212777</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.09833795013850409</v>
+        <v>-0.1007615700058582</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.08545397423814012</v>
+        <v>0.009292720702116654</v>
       </c>
     </row>
     <row r="8">
@@ -2401,16 +2401,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.3026315789473684</v>
+        <v>-0.36507936507936506</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.09345794392523357</v>
+        <v>0.44999999999999984</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1925925925925926</v>
+        <v>-0.17777777777777767</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.19767441860465118</v>
+        <v>0.01639344262295072</v>
       </c>
     </row>
     <row r="9">
@@ -2421,16 +2421,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.29579375848032563</v>
+        <v>-0.3682539682539682</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.09845559845559847</v>
+        <v>0.44162436548223366</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.18518518518518515</v>
+        <v>-0.19026548672566365</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.17808219178082185</v>
+        <v>0.009740259740259681</v>
       </c>
     </row>
     <row r="10">
@@ -2441,16 +2441,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.2909516380655227</v>
+        <v>-0.36684303350970016</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.09988901220865698</v>
+        <v>0.43589743589743596</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.17520215633423172</v>
+        <v>-0.19354838709677422</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.16097922848664686</v>
+        <v>0.008992805755395692</v>
       </c>
     </row>
     <row r="11">
@@ -2461,16 +2461,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6235167206040991</v>
+        <v>0.1652626362735381</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6629692832764504</v>
+        <v>0.40766666666666673</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6819541375872382</v>
+        <v>0.24157764995891537</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4977890082122553</v>
+        <v>0.3283828382838284</v>
       </c>
     </row>
     <row r="12">
@@ -2481,16 +2481,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>0.10958904109589039</v>
+        <v>-0.34448160535117056</v>
       </c>
       <c r="D12" t="n">
-        <v>0.387434554973822</v>
+        <v>0.6728395061728395</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3299999999999999</v>
+        <v>-0.1310679611650486</v>
       </c>
       <c r="F12" t="n">
-        <v>0.20857142857142838</v>
+        <v>0.19196428571428578</v>
       </c>
     </row>
     <row r="13">
@@ -2501,16 +2501,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.030263157894736832</v>
+        <v>-0.043707796193983996</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.018610271903323226</v>
+        <v>-0.03238916256157648</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.014927184466019391</v>
+        <v>-0.02096793855906375</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.014134780125642519</v>
+        <v>-0.014035087719298322</v>
       </c>
     </row>
     <row r="14">
@@ -2521,16 +2521,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.05353852823236155</v>
+        <v>-0.14308847342852946</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.051159765879037526</v>
+        <v>-0.13410067951740398</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.06154011384384064</v>
+        <v>-0.14885100074128974</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.06560726447219065</v>
+        <v>-0.08119601328903646</v>
       </c>
     </row>
     <row r="15">
@@ -2541,16 +2541,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.358695652173913</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6573426573426573</v>
+        <v>1.2848751835535976</v>
       </c>
       <c r="E15" t="n">
-        <v>0.933628318584071</v>
+        <v>0.7906976744186045</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4650112866817156</v>
+        <v>0.6989079563182525</v>
       </c>
     </row>
     <row r="16">
@@ -2561,16 +2561,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.10646347248576854</v>
+        <v>0.08952128443069678</v>
       </c>
       <c r="D16" t="n">
-        <v>0.05658243391714615</v>
+        <v>0.011766071912373808</v>
       </c>
       <c r="E16" t="n">
-        <v>0.03697971258681674</v>
+        <v>0.02028682068117373</v>
       </c>
       <c r="F16" t="n">
-        <v>0.029814852643503083</v>
+        <v>-0.014191855109241768</v>
       </c>
     </row>
     <row r="17">
@@ -2581,16 +2581,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.22107969151670945</v>
+        <v>-0.15217391304347822</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.08375209380234513</v>
+        <v>0.0</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.05323193916349817</v>
+        <v>-0.03246753246753249</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.07142857142857141</v>
+        <v>0.00628930817610059</v>
       </c>
     </row>
     <row r="18">
@@ -2601,16 +2601,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7270471464019849</v>
+        <v>0.1527254458678723</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7246511627906977</v>
+        <v>0.3862938970337539</v>
       </c>
       <c r="E18" t="n">
-        <v>0.7788125727590219</v>
+        <v>0.23596442468037793</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5629043853342919</v>
+        <v>0.3227603943420488</v>
       </c>
     </row>
     <row r="19">
@@ -2621,16 +2621,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.47058823529411764</v>
+        <v>-0.2</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.14705882352941177</v>
+        <v>0.3661971830985915</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0</v>
+        <v>0.16666666666666677</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.18181818181818188</v>
+        <v>1.2727272727272727</v>
       </c>
     </row>
     <row r="20">
@@ -2641,16 +2641,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.03440621531631512</v>
+        <v>-0.031602155805977514</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.06913455037187297</v>
+        <v>-0.021288949100058078</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.017571261226083504</v>
+        <v>-0.008671257332313222</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.039371438438956886</v>
+        <v>0.02426242236024836</v>
       </c>
     </row>
   </sheetData>
@@ -2692,16 +2692,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.12386706948640488</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.09311740890688261</v>
+        <v>0.0</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.11168032786885253</v>
+        <v>0.0</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.11807120324470471</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -2712,16 +2712,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1378839590443686</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.05607476635514011</v>
+        <v>0.0</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.10044642857142856</v>
+        <v>0.0</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.11163416274377945</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -2732,16 +2732,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.12794033275960995</v>
+        <v>0.0</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.08327501749475154</v>
+        <v>0.0</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.11190903650508674</v>
+        <v>0.0</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.11695906432748535</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -2752,16 +2752,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1229551451187336</v>
+        <v>0.0</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.08785046728971964</v>
+        <v>0.0</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.11152025249868489</v>
+        <v>0.0</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.11856400566839873</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -2772,16 +2772,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.24791086350974934</v>
+        <v>0.0</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.1409395973154362</v>
+        <v>0.0</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.17971014492753634</v>
+        <v>0.0</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.22601279317697226</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -2792,16 +2792,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.120923415170392</v>
+        <v>0.0</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.07603305785123968</v>
+        <v>0.0</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0945945945945947</v>
+        <v>0.0</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.11331351172778327</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
@@ -2812,16 +2812,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.2540983606557377</v>
+        <v>0.0</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.11578947368421055</v>
+        <v>0.0</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.17391304347826086</v>
+        <v>0.0</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.2251655629139073</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -2832,16 +2832,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.24190800681431013</v>
+        <v>0.0</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.12147505422993493</v>
+        <v>0.0</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.16967509025270755</v>
+        <v>0.0</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.2169680111265647</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
@@ -2852,16 +2852,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.23205506391347094</v>
+        <v>0.0</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.13135068153655513</v>
+        <v>0.0</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1671891327063741</v>
+        <v>0.0</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.20734693877551014</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -2872,16 +2872,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.08017334777898148</v>
+        <v>0.0</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.057191634656423365</v>
+        <v>0.0</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.060800790904597155</v>
+        <v>0.0</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0910458991723099</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="12">
@@ -2892,16 +2892,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.2712933753943218</v>
+        <v>0.0</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.17589576547231275</v>
+        <v>0.0</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.20312500000000006</v>
+        <v>0.0</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.2505050505050505</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -2912,16 +2912,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.03513022410660209</v>
+        <v>0.0</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.019123020706455465</v>
+        <v>0.0</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.01403808593750008</v>
+        <v>0.0</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.011384925781812808</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="14">
@@ -2932,16 +2932,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.015508395522388033</v>
+        <v>0.0</v>
       </c>
       <c r="D14" t="n">
-        <v>0.020378632581695304</v>
+        <v>0.0</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.0017736786094360373</v>
+        <v>0.0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.032736177342441004</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="15">
@@ -2952,16 +2952,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.188715953307393</v>
+        <v>0.0</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.10402684563758384</v>
+        <v>0.0</v>
       </c>
       <c r="E15" t="n">
-        <v>0.019438444924406006</v>
+        <v>0.0</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.13351498637602183</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="16">
@@ -2972,16 +2972,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.07682308232704019</v>
+        <v>0.0</v>
       </c>
       <c r="D16" t="n">
-        <v>0.030466301953524833</v>
+        <v>0.0</v>
       </c>
       <c r="E16" t="n">
-        <v>0.022615272949535734</v>
+        <v>0.0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.018483885610531072</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="17">
@@ -2992,16 +2992,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.182089552238806</v>
+        <v>0.0</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.06989247311827958</v>
+        <v>0.0</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.03952569169960478</v>
+        <v>0.0</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.044303797468354486</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
@@ -3012,16 +3012,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.056547619047619097</v>
+        <v>0.0</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.03595812471552125</v>
+        <v>0.0</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.03638368246968023</v>
+        <v>0.0</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.06636060100166943</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="19">
@@ -3032,16 +3032,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.41379310344827586</v>
+        <v>0.0</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.2000000000000001</v>
+        <v>0.0</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.11111111111111105</v>
+        <v>0.0</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.2222222222222222</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="20">
@@ -3052,16 +3052,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.02832574607991904</v>
+        <v>0.0</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.0482013113592061</v>
+        <v>0.0</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.010800842992623795</v>
+        <v>0.0</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.025187566988210078</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -3103,16 +3103,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.018244013683010363</v>
+        <v>-0.020481310803891466</v>
       </c>
       <c r="D2" t="n">
-        <v>0.10619803476946339</v>
+        <v>0.0</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.013269819666553299</v>
+        <v>-0.055804823331463756</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03562054743157109</v>
+        <v>-0.13854835571122795</v>
       </c>
     </row>
     <row r="3">
@@ -3123,16 +3123,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.008324084350721428</v>
+        <v>-0.0473026840287006</v>
       </c>
       <c r="D3" t="n">
-        <v>0.20423892100192675</v>
+        <v>-0.009154929577464823</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.004162330905307091</v>
+        <v>-0.09450679267572365</v>
       </c>
       <c r="F3" t="n">
-        <v>0.051546391752577365</v>
+        <v>-0.17800081933633763</v>
       </c>
     </row>
     <row r="4">
@@ -3143,16 +3143,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.011116051578479334</v>
+        <v>-0.033315981259760485</v>
       </c>
       <c r="D4" t="n">
-        <v>0.14126394052044614</v>
+        <v>-0.004124656278643501</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.01010101010101011</v>
+        <v>-0.07292563881711163</v>
       </c>
       <c r="F4" t="n">
-        <v>0.04216600088770532</v>
+        <v>-0.1560509554140127</v>
       </c>
     </row>
     <row r="5">
@@ -3163,16 +3163,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.013682092555331937</v>
+        <v>-0.026532715095311632</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1194274028629857</v>
+        <v>-0.0015865820489573401</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.012955182072829259</v>
+        <v>-0.05915492957746469</v>
       </c>
       <c r="F5" t="n">
-        <v>0.03773584905660376</v>
+        <v>-0.144481474220741</v>
       </c>
     </row>
     <row r="6">
@@ -3183,16 +3183,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.06532663316582928</v>
+        <v>0.0418794688457609</v>
       </c>
       <c r="D6" t="n">
-        <v>0.17408376963350794</v>
+        <v>0.021126760563380344</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.07011866235167212</v>
+        <v>0.061757719714964326</v>
       </c>
       <c r="F6" t="n">
-        <v>0.05412719891745608</v>
+        <v>-0.16817532158170556</v>
       </c>
     </row>
     <row r="7">
@@ -3203,16 +3203,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.025568980050575996</v>
+        <v>-0.036931277365315006</v>
       </c>
       <c r="D7" t="n">
-        <v>0.08936525612472149</v>
+        <v>-0.02466598150051382</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.021415973796926058</v>
+        <v>-0.04113858300436315</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0329183955739973</v>
+        <v>-0.1161242603550296</v>
       </c>
     </row>
     <row r="8">
@@ -3223,16 +3223,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.05714285714285713</v>
+        <v>-0.36531365313653136</v>
       </c>
       <c r="D8" t="n">
-        <v>0.18750000000000006</v>
+        <v>-0.3176206509539843</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.05098039215686271</v>
+        <v>-0.27009646302250795</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0724637681159421</v>
+        <v>-0.41935483870967744</v>
       </c>
     </row>
     <row r="9">
@@ -3243,16 +3243,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.05887681159420283</v>
+        <v>-0.1219715956558062</v>
       </c>
       <c r="D9" t="n">
-        <v>0.19007490636704105</v>
+        <v>-0.08207646439845678</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.06346749226006201</v>
+        <v>-0.10114030738720874</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06445312499999994</v>
+        <v>-0.2415902140672784</v>
       </c>
     </row>
     <row r="10">
@@ -3263,16 +3263,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.06032818532818525</v>
+        <v>-0.11000552791597568</v>
       </c>
       <c r="D10" t="n">
-        <v>0.18089944416371906</v>
+        <v>-0.05729653882132827</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0752458315519453</v>
+        <v>-0.07088186356073206</v>
       </c>
       <c r="F10" t="n">
-        <v>0.05530973451327439</v>
+        <v>-0.19503063308373048</v>
       </c>
     </row>
     <row r="11">
@@ -3283,16 +3283,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0.05404404960207293</v>
+        <v>1.0831556503198294</v>
       </c>
       <c r="D11" t="n">
-        <v>0.09895470383275275</v>
+        <v>0.4781976744186046</v>
       </c>
       <c r="E11" t="n">
-        <v>0.05434782608695648</v>
+        <v>0.9026548672566371</v>
       </c>
       <c r="F11" t="n">
-        <v>0.08183800100620485</v>
+        <v>0.267524115755627</v>
       </c>
     </row>
     <row r="12">
@@ -3303,16 +3303,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.07258834765998086</v>
+        <v>0.7201492537313433</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1384152457372117</v>
+        <v>0.38262910798122074</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.07749999999999992</v>
+        <v>0.7764705882352942</v>
       </c>
       <c r="F12" t="n">
-        <v>0.030769230769230795</v>
+        <v>0.0651465798045602</v>
       </c>
     </row>
     <row r="13">
@@ -3323,16 +3323,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.022936327798351447</v>
+        <v>0.0015628488501897263</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.017948096046568076</v>
+        <v>-0.025214966302579654</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.010233566096797438</v>
+        <v>-0.011958146487294556</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.008780768677126809</v>
+        <v>-0.047625144027653325</v>
       </c>
     </row>
     <row r="14">
@@ -3343,16 +3343,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.04729945669542996</v>
+        <v>-0.010397553516819558</v>
       </c>
       <c r="D14" t="n">
-        <v>5.042864346948511E-4</v>
+        <v>-0.007262684124386247</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.0368997472620051</v>
+        <v>-0.01412171086050992</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.04019746121297609</v>
+        <v>-0.030967078189300428</v>
       </c>
     </row>
     <row r="15">
@@ -3363,16 +3363,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.10671191553544492</v>
+        <v>1.5679611650485439</v>
       </c>
       <c r="D15" t="n">
-        <v>0.39526484751203855</v>
+        <v>0.8813056379821957</v>
       </c>
       <c r="E15" t="n">
-        <v>0.21423562412342212</v>
+        <v>1.225941422594142</v>
       </c>
       <c r="F15" t="n">
-        <v>0.31622581918673487</v>
+        <v>0.20491803278688514</v>
       </c>
     </row>
     <row r="16">
@@ -3383,16 +3383,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.04205636229387166</v>
+        <v>-0.1060418351779992</v>
       </c>
       <c r="D16" t="n">
-        <v>3.9455303539231176E-4</v>
+        <v>-0.031006067191886227</v>
       </c>
       <c r="E16" t="n">
-        <v>0.013253159896919893</v>
+        <v>0.008581825207702731</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.0032596305124025456</v>
+        <v>-0.004736736468856521</v>
       </c>
     </row>
     <row r="17">
@@ -3403,16 +3403,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.07441860465116266</v>
+        <v>0.15863141524105756</v>
       </c>
       <c r="D17" t="n">
-        <v>0.013245033112582702</v>
+        <v>0.100767754318618</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.030612244897959176</v>
+        <v>-0.04718693284936488</v>
       </c>
       <c r="F17" t="n">
-        <v>0.005649717514124259</v>
+        <v>-0.23408624229979466</v>
       </c>
     </row>
     <row r="18">
@@ -3423,16 +3423,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>0.04965883244882487</v>
+        <v>1.7040816326530615</v>
       </c>
       <c r="D18" t="n">
-        <v>0.09269863994273456</v>
+        <v>0.7046004842615011</v>
       </c>
       <c r="E18" t="n">
-        <v>0.052303429165223424</v>
+        <v>0.9203747072599532</v>
       </c>
       <c r="F18" t="n">
-        <v>0.07883888698041899</v>
+        <v>0.5635018495684339</v>
       </c>
     </row>
     <row r="19">
@@ -3443,16 +3443,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2000000000000001</v>
+        <v>-0.2884615384615384</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1260504201680672</v>
+        <v>0.9931506849315069</v>
       </c>
       <c r="E19" t="n">
-        <v>0.22222222222222232</v>
+        <v>0.0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8</v>
+        <v>2.666666666666667</v>
       </c>
     </row>
     <row r="20">
@@ -3463,16 +3463,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.012001454721784483</v>
+        <v>0.012467476149176013</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.002022585538513551</v>
+        <v>0.010906862745098063</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.004055548728032407</v>
+        <v>6.694934166481198E-4</v>
       </c>
       <c r="F20" t="n">
-        <v>0.004809343868086419</v>
+        <v>0.011914217633042108</v>
       </c>
     </row>
   </sheetData>
@@ -3514,16 +3514,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.05062205062205064</v>
+        <v>-0.04277062831188485</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.031156156156156266</v>
+        <v>0.04782237403928273</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.01414617716402823</v>
+        <v>0.07702020202020206</v>
       </c>
       <c r="F2" t="n">
-        <v>0.025995948683322025</v>
+        <v>-0.014170040485829972</v>
       </c>
     </row>
     <row r="3">
@@ -3534,16 +3534,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.04161073825503345</v>
+        <v>-0.028555431131019153</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.009248554913294743</v>
+        <v>0.17752808988764043</v>
       </c>
       <c r="E3" t="n">
-        <v>0.015408320493066126</v>
+        <v>0.16430412371134018</v>
       </c>
       <c r="F3" t="n">
-        <v>0.061716006021073785</v>
+        <v>0.07799074686054201</v>
       </c>
     </row>
     <row r="4">
@@ -3554,16 +3554,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.04771677783478709</v>
+        <v>-0.03434433541480826</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.024021352313167207</v>
+        <v>0.09531416400425985</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.003980891719745226</v>
+        <v>0.11016096579476863</v>
       </c>
       <c r="F4" t="n">
-        <v>0.040332147093712876</v>
+        <v>0.01877470355731224</v>
       </c>
     </row>
     <row r="5">
@@ -3574,16 +3574,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.04922515952597996</v>
+        <v>-0.038369304556354795</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.027966440271674123</v>
+        <v>0.06552044609665428</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.012798339674853118</v>
+        <v>0.082827406764961</v>
       </c>
       <c r="F5" t="n">
-        <v>0.029287226534933063</v>
+        <v>-0.004286326618088302</v>
       </c>
     </row>
     <row r="6">
@@ -3594,16 +3594,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.10620915032679737</v>
+        <v>-0.0654761904761905</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.07030129124820662</v>
+        <v>0.08803986710963466</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.025219298245613996</v>
+        <v>0.12727272727272726</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01795735129068467</v>
+        <v>-0.08306709265175724</v>
       </c>
     </row>
     <row r="7">
@@ -3614,16 +3614,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.057411907654920935</v>
+        <v>-0.024444444444444373</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.032538569424964935</v>
+        <v>0.04838221953432118</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.010958904109589078</v>
+        <v>0.0749846342962507</v>
       </c>
       <c r="F7" t="n">
-        <v>0.014790674354474847</v>
+        <v>-0.024992734670154015</v>
       </c>
     </row>
     <row r="8">
@@ -3634,16 +3634,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.09444444444444446</v>
+        <v>-0.029411764705882464</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.07281553398058259</v>
+        <v>0.19597989949748745</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.025925925925925897</v>
+        <v>0.1902173913043478</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03488372093023261</v>
+        <v>-0.03755868544600933</v>
       </c>
     </row>
     <row r="9">
@@ -3654,16 +3654,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.10348837209302317</v>
+        <v>-0.03380281690140838</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.06700507614213207</v>
+        <v>0.1450549450549451</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0222222222222222</v>
+        <v>0.17273795534665107</v>
       </c>
       <c r="F9" t="n">
-        <v>0.027397260273972605</v>
+        <v>-0.04428424304840383</v>
       </c>
     </row>
     <row r="10">
@@ -3674,16 +3674,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.107264086897488</v>
+        <v>-0.03859447004608301</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.06520450503852983</v>
+        <v>0.10942649967040213</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.019514516896715944</v>
+        <v>0.15400843881856544</v>
       </c>
       <c r="F10" t="n">
-        <v>0.020216267042783256</v>
+        <v>-0.05400372439478576</v>
       </c>
     </row>
     <row r="11">
@@ -3694,16 +3694,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.003205128205128233</v>
+        <v>-0.11863117870722435</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.030062111801242235</v>
+        <v>-0.1265619993591797</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.03102153724560362</v>
+        <v>-0.125230882896195</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.06037567084078705</v>
+        <v>-0.15123010130246012</v>
       </c>
     </row>
     <row r="12">
@@ -3714,16 +3714,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.10619469026548678</v>
+        <v>-0.13533834586466167</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.07525655644241727</v>
+        <v>-0.017964071856287317</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.03015075376884427</v>
+        <v>0.01929824561403503</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.0034904013961605377</v>
+        <v>-0.1725731895223421</v>
       </c>
     </row>
     <row r="13">
@@ -3734,16 +3734,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.038313685289595126</v>
+        <v>-0.03215011354129322</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.04792746113989641</v>
+        <v>-0.023339317773788237</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.019701419481155166</v>
+        <v>-0.01564964212058719</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.028834894613583212</v>
+        <v>-0.020405271361768413</v>
       </c>
     </row>
     <row r="14">
@@ -3754,16 +3754,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.04044585987261143</v>
+        <v>0.004040404040404016</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.03336791147994465</v>
+        <v>0.018035061167864772</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.020723504817306084</v>
+        <v>0.014320419383710507</v>
       </c>
       <c r="F14" t="n">
-        <v>0.02327746741154554</v>
+        <v>0.02453271028037387</v>
       </c>
     </row>
     <row r="15">
@@ -3774,16 +3774,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1138952164009111</v>
+        <v>-0.2678571428571429</v>
       </c>
       <c r="D15" t="n">
-        <v>0.18924581005586602</v>
+        <v>-0.25562372188139054</v>
       </c>
       <c r="E15" t="n">
-        <v>0.03293687099725532</v>
+        <v>-0.18825100133511344</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.07419505366308912</v>
+        <v>-0.28428927680798</v>
       </c>
     </row>
     <row r="16">
@@ -3794,16 +3794,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.05941500087673148</v>
+        <v>0.07521764544612793</v>
       </c>
       <c r="D16" t="n">
-        <v>0.020290166997661816</v>
+        <v>0.04479179288339593</v>
       </c>
       <c r="E16" t="n">
-        <v>0.028734211122787328</v>
+        <v>0.05571431257167572</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.022714879694635707</v>
+        <v>0.051067840345515564</v>
       </c>
     </row>
     <row r="17">
@@ -3814,16 +3814,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.12589928057553956</v>
+        <v>-0.22641509433962267</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.07692307692307705</v>
+        <v>-0.11090573012939012</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.052924791086350946</v>
+        <v>-0.09505703422053227</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0</v>
+        <v>-0.09493670886075957</v>
       </c>
     </row>
     <row r="18">
@@ -3834,16 +3834,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.015067805123053755</v>
+        <v>-0.09608540925266908</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.04591688462656215</v>
+        <v>-0.11455576559546321</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.04006063230835851</v>
+        <v>-0.12208800690250224</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.06663196251952111</v>
+        <v>-0.12062937062937068</v>
       </c>
     </row>
     <row r="19">
@@ -3854,16 +3854,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2000000000000001</v>
+        <v>-0.06250000000000003</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.06451612903225809</v>
+        <v>-0.75</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.18750000000000008</v>
+        <v>-0.375</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6666666666666666</v>
+        <v>-0.2857142857142857</v>
       </c>
     </row>
     <row r="20">
@@ -3874,16 +3874,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.025724683147195473</v>
+        <v>-0.0325277596342259</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.03677793324005591</v>
+        <v>-0.07859778597785982</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.010642341315089272</v>
+        <v>-0.028306878306878273</v>
       </c>
       <c r="F20" t="n">
-        <v>0.04120824164832957</v>
+        <v>-0.06290555155010803</v>
       </c>
     </row>
   </sheetData>
@@ -3925,16 +3925,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.04277062831188485</v>
+        <v>-0.1660839160839161</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04782237403928273</v>
+        <v>-0.07484076433121019</v>
       </c>
       <c r="E2" t="n">
-        <v>0.07702020202020206</v>
+        <v>-0.10225140712945598</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.014170040485829972</v>
+        <v>-0.08454312553373179</v>
       </c>
     </row>
     <row r="3">
@@ -3945,16 +3945,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.028555431131019153</v>
+        <v>-0.26457399103139007</v>
       </c>
       <c r="D3" t="n">
-        <v>0.17752808988764043</v>
+        <v>-0.19405940594059404</v>
       </c>
       <c r="E3" t="n">
-        <v>0.16430412371134018</v>
+        <v>-0.20720221606648195</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07799074686054201</v>
+        <v>-0.19778481012658217</v>
       </c>
     </row>
     <row r="4">
@@ -3965,16 +3965,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.03434433541480826</v>
+        <v>-0.20612813370473534</v>
       </c>
       <c r="D4" t="n">
-        <v>0.09531416400425985</v>
+        <v>-0.12339930151338764</v>
       </c>
       <c r="E4" t="n">
-        <v>0.11016096579476863</v>
+        <v>-0.14883955600403634</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01877470355731224</v>
+        <v>-0.13102480112306972</v>
       </c>
     </row>
     <row r="5">
@@ -3985,16 +3985,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.038369304556354795</v>
+        <v>-0.1788109074653554</v>
       </c>
       <c r="D5" t="n">
-        <v>0.06552044609665428</v>
+        <v>-0.09306167400881056</v>
       </c>
       <c r="E5" t="n">
-        <v>0.082827406764961</v>
+        <v>-0.11021377672209026</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.004286326618088302</v>
+        <v>-0.09784993418165856</v>
       </c>
     </row>
     <row r="6">
@@ -4005,16 +4005,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.0654761904761905</v>
+        <v>-0.21282051282051279</v>
       </c>
       <c r="D6" t="n">
-        <v>0.08803986710963466</v>
+        <v>0.003472222222222201</v>
       </c>
       <c r="E6" t="n">
-        <v>0.12727272727272726</v>
+        <v>-0.08115942028985518</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.08306709265175724</v>
+        <v>-0.08639308855291584</v>
       </c>
     </row>
     <row r="7">
@@ -4025,16 +4025,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.024444444444444373</v>
+        <v>-0.15319426336375502</v>
       </c>
       <c r="D7" t="n">
-        <v>0.04838221953432118</v>
+        <v>-0.05499612703330748</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0749846342962507</v>
+        <v>-0.09833795013850409</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.024992734670154015</v>
+        <v>-0.08545397423814012</v>
       </c>
     </row>
     <row r="8">
@@ -4045,16 +4045,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.029411764705882464</v>
+        <v>-0.3026315789473684</v>
       </c>
       <c r="D8" t="n">
-        <v>0.19597989949748745</v>
+        <v>-0.09345794392523357</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1902173913043478</v>
+        <v>-0.1925925925925926</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.03755868544600933</v>
+        <v>-0.19767441860465118</v>
       </c>
     </row>
     <row r="9">
@@ -4065,16 +4065,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.03380281690140838</v>
+        <v>-0.29579375848032563</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1450549450549451</v>
+        <v>-0.09845559845559847</v>
       </c>
       <c r="E9" t="n">
-        <v>0.17273795534665107</v>
+        <v>-0.18518518518518515</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.04428424304840383</v>
+        <v>-0.17808219178082185</v>
       </c>
     </row>
     <row r="10">
@@ -4085,16 +4085,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.03859447004608301</v>
+        <v>-0.2909516380655227</v>
       </c>
       <c r="D10" t="n">
-        <v>0.10942649967040213</v>
+        <v>-0.09988901220865698</v>
       </c>
       <c r="E10" t="n">
-        <v>0.15400843881856544</v>
+        <v>-0.17520215633423172</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.05400372439478576</v>
+        <v>-0.16097922848664686</v>
       </c>
     </row>
     <row r="11">
@@ -4105,16 +4105,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.11863117870722435</v>
+        <v>0.6235167206040991</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.1265619993591797</v>
+        <v>0.6629692832764504</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.125230882896195</v>
+        <v>0.6819541375872382</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.15123010130246012</v>
+        <v>0.4977890082122553</v>
       </c>
     </row>
     <row r="12">
@@ -4125,16 +4125,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.13533834586466167</v>
+        <v>0.10958904109589039</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.017964071856287317</v>
+        <v>0.387434554973822</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01929824561403503</v>
+        <v>0.3299999999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.1725731895223421</v>
+        <v>0.20857142857142838</v>
       </c>
     </row>
     <row r="13">
@@ -4145,16 +4145,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.03215011354129322</v>
+        <v>-0.030263157894736832</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.023339317773788237</v>
+        <v>-0.018610271903323226</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.01564964212058719</v>
+        <v>-0.014927184466019391</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.020405271361768413</v>
+        <v>-0.014134780125642519</v>
       </c>
     </row>
     <row r="14">
@@ -4165,16 +4165,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>0.004040404040404016</v>
+        <v>-0.05353852823236155</v>
       </c>
       <c r="D14" t="n">
-        <v>0.018035061167864772</v>
+        <v>-0.051159765879037526</v>
       </c>
       <c r="E14" t="n">
-        <v>0.014320419383710507</v>
+        <v>-0.06154011384384064</v>
       </c>
       <c r="F14" t="n">
-        <v>0.02453271028037387</v>
+        <v>-0.06560726447219065</v>
       </c>
     </row>
     <row r="15">
@@ -4185,16 +4185,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.2678571428571429</v>
+        <v>0.358695652173913</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.25562372188139054</v>
+        <v>0.6573426573426573</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.18825100133511344</v>
+        <v>0.933628318584071</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.28428927680798</v>
+        <v>0.4650112866817156</v>
       </c>
     </row>
     <row r="16">
@@ -4205,16 +4205,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.07521764544612793</v>
+        <v>0.10646347248576854</v>
       </c>
       <c r="D16" t="n">
-        <v>0.04479179288339593</v>
+        <v>0.05658243391714615</v>
       </c>
       <c r="E16" t="n">
-        <v>0.05571431257167572</v>
+        <v>0.03697971258681674</v>
       </c>
       <c r="F16" t="n">
-        <v>0.051067840345515564</v>
+        <v>0.029814852643503083</v>
       </c>
     </row>
     <row r="17">
@@ -4225,16 +4225,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.22641509433962267</v>
+        <v>-0.22107969151670945</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.11090573012939012</v>
+        <v>-0.08375209380234513</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.09505703422053227</v>
+        <v>-0.05323193916349817</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.09493670886075957</v>
+        <v>-0.07142857142857141</v>
       </c>
     </row>
     <row r="18">
@@ -4245,16 +4245,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.09608540925266908</v>
+        <v>0.7270471464019849</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.11455576559546321</v>
+        <v>0.7246511627906977</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.12208800690250224</v>
+        <v>0.7788125727590219</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.12062937062937068</v>
+        <v>0.5629043853342919</v>
       </c>
     </row>
     <row r="19">
@@ -4265,16 +4265,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.06250000000000003</v>
+        <v>-0.47058823529411764</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.75</v>
+        <v>-0.14705882352941177</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.375</v>
+        <v>0.0</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.2857142857142857</v>
+        <v>-0.18181818181818188</v>
       </c>
     </row>
     <row r="20">
@@ -4285,16 +4285,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.0325277596342259</v>
+        <v>-0.03440621531631512</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.07859778597785982</v>
+        <v>-0.06913455037187297</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.028306878306878273</v>
+        <v>-0.017571261226083504</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.06290555155010803</v>
+        <v>-0.039371438438956886</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
produce comparisons between seg indices
</commit_message>
<xml_diff>
--- a/tables/change_in_segs.xlsx
+++ b/tables/change_in_segs.xlsx
@@ -16,12 +16,13 @@
     <sheet name="Pensioner" r:id="rId10" sheetId="8"/>
     <sheet name="Poor Health" r:id="rId11" sheetId="9"/>
     <sheet name="Single" r:id="rId12" sheetId="10"/>
+    <sheet name="Student" r:id="rId13" sheetId="11"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="43">
   <si>
     <t>index</t>
   </si>
@@ -1014,6 +1015,417 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-0.015846538782318703</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.03748594277146074</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.06652719665271963</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-0.09214501510574023</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-0.019643608811561686</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.04000000000000009</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-0.07076006806579702</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-0.09690904484418547</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.017311182465447546</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.03845670478823673</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.06856821694534207</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-0.09429437010855843</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.016441410059913657</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.0380904648540283</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-0.0668064290705801</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-0.092891353667759</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.010000000000000047</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.03558627752176145</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.0793795620437955</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-0.1138034304383338</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-0.01492537313432841</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.02247314185485635</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-0.0417246175243394</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-0.054319371727748644</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-0.05446082234290134</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-0.1247392574050897</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-0.17879558948261245</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-0.2241743725231175</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.03050524308865583</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.057486631016042795</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-0.09642857142857134</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-0.12491035142242414</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-0.023980815347721843</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.03372066529961275</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-0.05892504930966477</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-0.07622913847541722</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.275</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.15840893230983946</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.09799382716049396</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.21353065539112046</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.24580152671755728</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.13283018867924531</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.06510416666666673</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.16365688487584648</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="n">
+        <v>3.0364372469632284E-4</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.010232558139534904</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.013215400624349567</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-0.04394211471427059</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0013098236775818315</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-7.014730934963763E-4</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.004218137993371479</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.39292364990689027</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.25823045267489725</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.1164215686274509</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.36988543371522087</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.010991102440881143</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.032104492187499986</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.1719641779963807</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.2704822975646361</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-0.09491114701130854</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.007417873542917664</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.14880144730890993</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-0.25226757369614516</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.38888888888888884</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.3008130081300813</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.19540229885057475</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.36038186157517904</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-0.2626262626262627</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.061312607944732256</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1.7567567567567568</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2.9787234042553195</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.0019120458891013512</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.002562788313685349</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.004596527068437128</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-0.015537332757876532</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
@@ -2692,16 +3104,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>-0.0630372492836676</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>0.041751944330740955</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0</v>
+        <v>-0.02828989192625545</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0</v>
+        <v>0.06989779096604021</v>
       </c>
     </row>
     <row r="3">
@@ -2712,16 +3124,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0</v>
+        <v>-0.0725933719095212</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0</v>
+        <v>0.033609352167559614</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0</v>
+        <v>-0.047235023041474776</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0</v>
+        <v>0.03525523319867792</v>
       </c>
     </row>
     <row r="4">
@@ -2732,16 +3144,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0</v>
+        <v>-0.06706204379562052</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0</v>
+        <v>0.03883495145631069</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0</v>
+        <v>-0.03721571330117172</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0</v>
+        <v>0.05463347164591971</v>
       </c>
     </row>
     <row r="5">
@@ -2752,16 +3164,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>-0.0701606086221471</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0</v>
+        <v>0.038299663299663285</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0</v>
+        <v>-0.02997099581050606</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0</v>
+        <v>0.06423553027768483</v>
       </c>
     </row>
     <row r="6">
@@ -2772,16 +3184,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>-0.04267161410018559</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0</v>
+        <v>0.05987055016181233</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0</v>
+        <v>-0.013771186440677919</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0</v>
+        <v>0.21515892420537902</v>
       </c>
     </row>
     <row r="7">
@@ -2792,16 +3204,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>-0.05942376950780307</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0</v>
+        <v>0.019499417927823</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0</v>
+        <v>-0.022898961284230374</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0</v>
+        <v>0.06167400881057269</v>
       </c>
     </row>
     <row r="8">
@@ -2812,16 +3224,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0</v>
+        <v>-0.15300546448087435</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0</v>
+        <v>0.025773195876288683</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0</v>
+        <v>-0.03793103448275863</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0</v>
+        <v>0.12546125461254615</v>
       </c>
     </row>
     <row r="9">
@@ -2832,16 +3244,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0</v>
+        <v>-0.1152073732718895</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0</v>
+        <v>0.021298174442190718</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0</v>
+        <v>-0.04664310954063601</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0</v>
+        <v>0.12720588235294103</v>
       </c>
     </row>
     <row r="10">
@@ -2852,16 +3264,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0</v>
+        <v>-0.08175675675675675</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0</v>
+        <v>0.011647254575707259</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0</v>
+        <v>-0.05378973105134481</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0</v>
+        <v>0.12186084808563201</v>
       </c>
     </row>
     <row r="11">
@@ -2872,16 +3284,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0</v>
+        <v>0.3161693936477382</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0</v>
+        <v>0.24127906976744193</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0</v>
+        <v>0.22485422740524796</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0</v>
+        <v>0.45116279069767456</v>
       </c>
     </row>
     <row r="12">
@@ -2892,16 +3304,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0</v>
+        <v>0.17721518987341778</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0</v>
+        <v>0.08316633266533068</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0</v>
+        <v>0.4921383647798741</v>
       </c>
     </row>
     <row r="13">
@@ -2912,16 +3324,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0</v>
+        <v>0.036728563626433536</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0</v>
+        <v>-0.02260317460317451</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0</v>
+        <v>0.0012208521548040543</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0</v>
+        <v>-0.002864919066036387</v>
       </c>
     </row>
     <row r="14">
@@ -2932,16 +3344,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0</v>
+        <v>-0.013667117726657643</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0</v>
+        <v>-0.007851797325481625</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0</v>
+        <v>-0.007304983042003573</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0</v>
+        <v>-0.019829059829059796</v>
       </c>
     </row>
     <row r="15">
@@ -2952,16 +3364,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0</v>
+        <v>0.5373711340206185</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0</v>
+        <v>0.6246458923512749</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0</v>
+        <v>0.29635145197319435</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0</v>
+        <v>0.6837146702557197</v>
       </c>
     </row>
     <row r="16">
@@ -2972,16 +3384,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0</v>
+        <v>-0.09566849552411205</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0</v>
+        <v>-0.05856860434541258</v>
       </c>
       <c r="E16" t="n">
-        <v>0.0</v>
+        <v>-0.06714445688689816</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0</v>
+        <v>-0.09791099182823271</v>
       </c>
     </row>
     <row r="17">
@@ -2992,16 +3404,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0</v>
+        <v>0.41064638783269963</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>0.19811320754716985</v>
       </c>
       <c r="E17" t="n">
-        <v>0.0</v>
+        <v>0.019880715705765425</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0</v>
+        <v>0.12451361867704272</v>
       </c>
     </row>
     <row r="18">
@@ -3012,16 +3424,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0</v>
+        <v>0.3658675799086759</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0</v>
+        <v>0.2915407854984896</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0</v>
+        <v>0.2792718245759205</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0</v>
+        <v>0.4772162386081192</v>
       </c>
     </row>
     <row r="19">
@@ -3035,13 +3447,13 @@
         <v>0.0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0</v>
+        <v>0.09844559585492221</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0</v>
+        <v>0.14814814814814806</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0</v>
+        <v>1.9411764705882353</v>
       </c>
     </row>
     <row r="20">
@@ -3052,16 +3464,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0</v>
+        <v>0.0484173819742488</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0</v>
+        <v>0.08197029516826465</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0</v>
+        <v>0.0261437908496732</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0</v>
+        <v>0.11039603960396052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
produce new comparisons between segregation measure changes using revised version of good health categorisation; and employed and inactive tables
</commit_message>
<xml_diff>
--- a/tables/change_in_segs.xlsx
+++ b/tables/change_in_segs.xlsx
@@ -6,23 +6,25 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Grade 1 or 2" r:id="rId3" sheetId="1"/>
-    <sheet name="LLTI" r:id="rId4" sheetId="2"/>
-    <sheet name="No Car" r:id="rId5" sheetId="3"/>
-    <sheet name="Non-house" r:id="rId6" sheetId="4"/>
-    <sheet name="Non-religious" r:id="rId7" sheetId="5"/>
-    <sheet name="Not Scottish" r:id="rId8" sheetId="6"/>
-    <sheet name="Not White" r:id="rId9" sheetId="7"/>
-    <sheet name="Pensioner" r:id="rId10" sheetId="8"/>
-    <sheet name="Poor Health" r:id="rId11" sheetId="9"/>
-    <sheet name="Single" r:id="rId12" sheetId="10"/>
-    <sheet name="Student" r:id="rId13" sheetId="11"/>
+    <sheet name="Employed" r:id="rId3" sheetId="1"/>
+    <sheet name="Grade 1 or 2" r:id="rId4" sheetId="2"/>
+    <sheet name="Inactive" r:id="rId5" sheetId="3"/>
+    <sheet name="LLTI" r:id="rId6" sheetId="4"/>
+    <sheet name="No Car" r:id="rId7" sheetId="5"/>
+    <sheet name="Non-house" r:id="rId8" sheetId="6"/>
+    <sheet name="Non-religious" r:id="rId9" sheetId="7"/>
+    <sheet name="Not Scottish" r:id="rId10" sheetId="8"/>
+    <sheet name="Not White" r:id="rId11" sheetId="9"/>
+    <sheet name="Pensioner" r:id="rId12" sheetId="10"/>
+    <sheet name="Poor Health" r:id="rId13" sheetId="11"/>
+    <sheet name="Single" r:id="rId14" sheetId="12"/>
+    <sheet name="Student" r:id="rId15" sheetId="13"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="43">
   <si>
     <t>index</t>
   </si>
@@ -227,16 +229,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.05062205062205064</v>
+        <v>-0.052414605418139096</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.031156156156156266</v>
+        <v>-0.025130890052356015</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.01414617716402823</v>
+        <v>-0.020172910662824065</v>
       </c>
       <c r="F2" t="n">
-        <v>0.025995948683322025</v>
+        <v>-0.21376811594202896</v>
       </c>
     </row>
     <row r="3">
@@ -247,16 +249,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.04161073825503345</v>
+        <v>-0.041144901610017826</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.009248554913294743</v>
+        <v>0.07776669990029912</v>
       </c>
       <c r="E3" t="n">
-        <v>0.015408320493066126</v>
+        <v>0.06571741511500538</v>
       </c>
       <c r="F3" t="n">
-        <v>0.061716006021073785</v>
+        <v>-0.23741007194244598</v>
       </c>
     </row>
     <row r="4">
@@ -267,16 +269,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.04771677783478709</v>
+        <v>-0.045422781271837916</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.024021352313167207</v>
+        <v>0.00802139037433141</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.003980891719745226</v>
+        <v>0.005154639175257777</v>
       </c>
       <c r="F4" t="n">
-        <v>0.040332147093712876</v>
+        <v>-0.22278623801466443</v>
       </c>
     </row>
     <row r="5">
@@ -287,16 +289,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.04922515952597996</v>
+        <v>-0.051186017478152386</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.027966440271674123</v>
+        <v>-0.014359563469270547</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.012798339674853118</v>
+        <v>-0.015615615615615728</v>
       </c>
       <c r="F5" t="n">
-        <v>0.029287226534933063</v>
+        <v>-0.21686746987951802</v>
       </c>
     </row>
     <row r="6">
@@ -307,16 +309,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.10620915032679737</v>
+        <v>0.12721893491124278</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.07030129124820662</v>
+        <v>0.15827338129496407</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.025219298245613996</v>
+        <v>0.043927648578811374</v>
       </c>
       <c r="F6" t="n">
-        <v>0.01795735129068467</v>
+        <v>-0.32452830188679244</v>
       </c>
     </row>
     <row r="7">
@@ -327,16 +329,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.057411907654920935</v>
+        <v>-0.027265100671140963</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.032538569424964935</v>
+        <v>0.009822440498677715</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.010958904109589078</v>
+        <v>-0.018488745980707367</v>
       </c>
       <c r="F7" t="n">
-        <v>0.014790674354474847</v>
+        <v>-0.19505766062602967</v>
       </c>
     </row>
     <row r="8">
@@ -347,16 +349,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.09444444444444446</v>
+        <v>0.23762376237623775</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.07281553398058259</v>
+        <v>0.26016260162601623</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.025925925925925897</v>
+        <v>0.07499999999999998</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03488372093023261</v>
+        <v>-0.3096774193548387</v>
       </c>
     </row>
     <row r="9">
@@ -367,16 +369,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.10348837209302317</v>
+        <v>0.1218487394957983</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.06700507614213207</v>
+        <v>0.16551724137931018</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0222222222222222</v>
+        <v>0.04066543438077635</v>
       </c>
       <c r="F9" t="n">
-        <v>0.027397260273972605</v>
+        <v>-0.3206002728512961</v>
       </c>
     </row>
     <row r="10">
@@ -387,16 +389,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.107264086897488</v>
+        <v>0.0404411764705882</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.06520450503852983</v>
+        <v>0.09778225806451614</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.019514516896715944</v>
+        <v>0.0066666666666667035</v>
       </c>
       <c r="F10" t="n">
-        <v>0.020216267042783256</v>
+        <v>-0.3224</v>
       </c>
     </row>
     <row r="11">
@@ -407,16 +409,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.003205128205128233</v>
+        <v>0.04076958314246441</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.030062111801242235</v>
+        <v>0.02792506185931431</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.03102153724560362</v>
+        <v>-0.0030134813639966724</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.06037567084078705</v>
+        <v>0.031645569620253194</v>
       </c>
     </row>
     <row r="12">
@@ -427,16 +429,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.10619469026548678</v>
+        <v>0.12244897959183677</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.07525655644241727</v>
+        <v>0.13978494623655915</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.03015075376884427</v>
+        <v>0.05490196078431381</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.0034904013961605377</v>
+        <v>-0.3253521126760563</v>
       </c>
     </row>
     <row r="13">
@@ -447,16 +449,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.038313685289595126</v>
+        <v>-0.03174196851401516</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.04792746113989641</v>
+        <v>-0.03674974567650056</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.019701419481155166</v>
+        <v>-0.016260162601626004</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.028834894613583212</v>
+        <v>-0.022895125553914427</v>
       </c>
     </row>
     <row r="14">
@@ -467,16 +469,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.04044585987261143</v>
+        <v>-0.10416666666666659</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.03336791147994465</v>
+        <v>-0.06080502426491575</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.020723504817306084</v>
+        <v>-0.02035475428903753</v>
       </c>
       <c r="F14" t="n">
-        <v>0.02327746741154554</v>
+        <v>-0.08685685175751405</v>
       </c>
     </row>
     <row r="15">
@@ -487,16 +489,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1138952164009111</v>
+        <v>0.2922155688622754</v>
       </c>
       <c r="D15" t="n">
-        <v>0.18924581005586602</v>
+        <v>0.43872017353579157</v>
       </c>
       <c r="E15" t="n">
-        <v>0.03293687099725532</v>
+        <v>0.37303058387395743</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.07419505366308912</v>
+        <v>0.21512195121951222</v>
       </c>
     </row>
     <row r="16">
@@ -507,16 +509,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.05941500087673148</v>
+        <v>0.02702857113178258</v>
       </c>
       <c r="D16" t="n">
-        <v>0.020290166997661816</v>
+        <v>0.001772431153305923</v>
       </c>
       <c r="E16" t="n">
-        <v>0.028734211122787328</v>
+        <v>-0.0031526453560578056</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.022714879694635707</v>
+        <v>-0.030930911019758707</v>
       </c>
     </row>
     <row r="17">
@@ -527,16 +529,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.12589928057553956</v>
+        <v>-0.04897959183673468</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.07692307692307705</v>
+        <v>-0.021126760563380236</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.052924791086350946</v>
+        <v>0.014285714285714323</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0</v>
+        <v>0.029197080291970753</v>
       </c>
     </row>
     <row r="18">
@@ -547,16 +549,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.015067805123053755</v>
+        <v>0.02949852507374634</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.04591688462656215</v>
+        <v>0.014058453570107383</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.04006063230835851</v>
+        <v>-0.011186770428015592</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.06663196251952111</v>
+        <v>0.04148148148148143</v>
       </c>
     </row>
     <row r="19">
@@ -567,16 +569,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2000000000000001</v>
+        <v>-0.16666666666666663</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.06451612903225809</v>
+        <v>0.30769230769230765</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.18750000000000008</v>
+        <v>0.0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.8888888888888888</v>
       </c>
     </row>
     <row r="20">
@@ -587,16 +589,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.025724683147195473</v>
+        <v>-0.013230571612074471</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.03677793324005591</v>
+        <v>0.0010466820180029316</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.010642341315089272</v>
+        <v>0.0027533761636291997</v>
       </c>
       <c r="F20" t="n">
-        <v>0.04120824164832957</v>
+        <v>0.06130903065451524</v>
       </c>
     </row>
   </sheetData>
@@ -638,16 +640,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.018244013683010363</v>
+        <v>-0.04277062831188485</v>
       </c>
       <c r="D2" t="n">
-        <v>0.10619803476946339</v>
+        <v>0.04782237403928273</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.013269819666553299</v>
+        <v>0.07702020202020206</v>
       </c>
       <c r="F2" t="n">
-        <v>0.03562054743157109</v>
+        <v>-0.014170040485829972</v>
       </c>
     </row>
     <row r="3">
@@ -658,16 +660,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.008324084350721428</v>
+        <v>-0.028555431131019153</v>
       </c>
       <c r="D3" t="n">
-        <v>0.20423892100192675</v>
+        <v>0.17752808988764043</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.004162330905307091</v>
+        <v>0.16430412371134018</v>
       </c>
       <c r="F3" t="n">
-        <v>0.051546391752577365</v>
+        <v>0.07799074686054201</v>
       </c>
     </row>
     <row r="4">
@@ -678,16 +680,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.011116051578479334</v>
+        <v>-0.03434433541480826</v>
       </c>
       <c r="D4" t="n">
-        <v>0.14126394052044614</v>
+        <v>0.09531416400425985</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.01010101010101011</v>
+        <v>0.11016096579476863</v>
       </c>
       <c r="F4" t="n">
-        <v>0.04216600088770532</v>
+        <v>0.01877470355731224</v>
       </c>
     </row>
     <row r="5">
@@ -698,16 +700,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.013682092555331937</v>
+        <v>-0.038369304556354795</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1194274028629857</v>
+        <v>0.06552044609665428</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.012955182072829259</v>
+        <v>0.082827406764961</v>
       </c>
       <c r="F5" t="n">
-        <v>0.03773584905660376</v>
+        <v>-0.004286326618088302</v>
       </c>
     </row>
     <row r="6">
@@ -718,16 +720,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.06532663316582928</v>
+        <v>-0.0654761904761905</v>
       </c>
       <c r="D6" t="n">
-        <v>0.17408376963350794</v>
+        <v>0.08803986710963466</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.07011866235167212</v>
+        <v>0.12727272727272726</v>
       </c>
       <c r="F6" t="n">
-        <v>0.05412719891745608</v>
+        <v>-0.08306709265175724</v>
       </c>
     </row>
     <row r="7">
@@ -738,16 +740,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.025568980050575996</v>
+        <v>-0.024444444444444373</v>
       </c>
       <c r="D7" t="n">
-        <v>0.08936525612472149</v>
+        <v>0.04838221953432118</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.021415973796926058</v>
+        <v>0.0749846342962507</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0329183955739973</v>
+        <v>-0.024992734670154015</v>
       </c>
     </row>
     <row r="8">
@@ -758,16 +760,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.05714285714285713</v>
+        <v>-0.029411764705882464</v>
       </c>
       <c r="D8" t="n">
-        <v>0.18750000000000006</v>
+        <v>0.19597989949748745</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.05098039215686271</v>
+        <v>0.1902173913043478</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0724637681159421</v>
+        <v>-0.03755868544600933</v>
       </c>
     </row>
     <row r="9">
@@ -778,16 +780,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.05887681159420283</v>
+        <v>-0.03380281690140838</v>
       </c>
       <c r="D9" t="n">
-        <v>0.19007490636704105</v>
+        <v>0.1450549450549451</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.06346749226006201</v>
+        <v>0.17273795534665107</v>
       </c>
       <c r="F9" t="n">
-        <v>0.06445312499999994</v>
+        <v>-0.04428424304840383</v>
       </c>
     </row>
     <row r="10">
@@ -798,16 +800,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.06032818532818525</v>
+        <v>-0.03859447004608301</v>
       </c>
       <c r="D10" t="n">
-        <v>0.18089944416371906</v>
+        <v>0.10942649967040213</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0752458315519453</v>
+        <v>0.15400843881856544</v>
       </c>
       <c r="F10" t="n">
-        <v>0.05530973451327439</v>
+        <v>-0.05400372439478576</v>
       </c>
     </row>
     <row r="11">
@@ -818,16 +820,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0.05404404960207293</v>
+        <v>-0.11863117870722435</v>
       </c>
       <c r="D11" t="n">
-        <v>0.09895470383275275</v>
+        <v>-0.1265619993591797</v>
       </c>
       <c r="E11" t="n">
-        <v>0.05434782608695648</v>
+        <v>-0.125230882896195</v>
       </c>
       <c r="F11" t="n">
-        <v>0.08183800100620485</v>
+        <v>-0.15123010130246012</v>
       </c>
     </row>
     <row r="12">
@@ -838,16 +840,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.07258834765998086</v>
+        <v>-0.13533834586466167</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1384152457372117</v>
+        <v>-0.017964071856287317</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.07749999999999992</v>
+        <v>0.01929824561403503</v>
       </c>
       <c r="F12" t="n">
-        <v>0.030769230769230795</v>
+        <v>-0.1725731895223421</v>
       </c>
     </row>
     <row r="13">
@@ -858,16 +860,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.022936327798351447</v>
+        <v>-0.03215011354129322</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.017948096046568076</v>
+        <v>-0.023339317773788237</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.010233566096797438</v>
+        <v>-0.01564964212058719</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.008780768677126809</v>
+        <v>-0.020405271361768413</v>
       </c>
     </row>
     <row r="14">
@@ -878,16 +880,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.04729945669542996</v>
+        <v>0.004040404040404016</v>
       </c>
       <c r="D14" t="n">
-        <v>5.042864346948511E-4</v>
+        <v>0.018035061167864772</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.0368997472620051</v>
+        <v>0.014320419383710507</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.04019746121297609</v>
+        <v>0.02453271028037387</v>
       </c>
     </row>
     <row r="15">
@@ -898,16 +900,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.10671191553544492</v>
+        <v>-0.2678571428571429</v>
       </c>
       <c r="D15" t="n">
-        <v>0.39526484751203855</v>
+        <v>-0.25562372188139054</v>
       </c>
       <c r="E15" t="n">
-        <v>0.21423562412342212</v>
+        <v>-0.18825100133511344</v>
       </c>
       <c r="F15" t="n">
-        <v>0.31622581918673487</v>
+        <v>-0.28428927680798</v>
       </c>
     </row>
     <row r="16">
@@ -918,16 +920,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.04205636229387166</v>
+        <v>0.07521764544612793</v>
       </c>
       <c r="D16" t="n">
-        <v>3.9455303539231176E-4</v>
+        <v>0.04479179288339593</v>
       </c>
       <c r="E16" t="n">
-        <v>0.013253159896919893</v>
+        <v>0.05571431257167572</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.0032596305124025456</v>
+        <v>0.051067840345515564</v>
       </c>
     </row>
     <row r="17">
@@ -938,16 +940,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.07441860465116266</v>
+        <v>-0.22641509433962267</v>
       </c>
       <c r="D17" t="n">
-        <v>0.013245033112582702</v>
+        <v>-0.11090573012939012</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.030612244897959176</v>
+        <v>-0.09505703422053227</v>
       </c>
       <c r="F17" t="n">
-        <v>0.005649717514124259</v>
+        <v>-0.09493670886075957</v>
       </c>
     </row>
     <row r="18">
@@ -958,16 +960,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>0.04965883244882487</v>
+        <v>-0.09608540925266908</v>
       </c>
       <c r="D18" t="n">
-        <v>0.09269863994273456</v>
+        <v>-0.11455576559546321</v>
       </c>
       <c r="E18" t="n">
-        <v>0.052303429165223424</v>
+        <v>-0.12208800690250224</v>
       </c>
       <c r="F18" t="n">
-        <v>0.07883888698041899</v>
+        <v>-0.12062937062937068</v>
       </c>
     </row>
     <row r="19">
@@ -978,16 +980,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2000000000000001</v>
+        <v>-0.06250000000000003</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1260504201680672</v>
+        <v>-0.75</v>
       </c>
       <c r="E19" t="n">
-        <v>0.22222222222222232</v>
+        <v>-0.375</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8</v>
+        <v>-0.2857142857142857</v>
       </c>
     </row>
     <row r="20">
@@ -998,16 +1000,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.012001454721784483</v>
+        <v>-0.0325277596342259</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.002022585538513551</v>
+        <v>-0.07859778597785982</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.004055548728032407</v>
+        <v>-0.028306878306878273</v>
       </c>
       <c r="F20" t="n">
-        <v>0.004809343868086419</v>
+        <v>-0.06290555155010803</v>
       </c>
     </row>
   </sheetData>
@@ -1049,6 +1051,828 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
+        <v>0.0642482517482517</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.14649681528662412</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.13555347091932463</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.08326216908625103</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.13901345291479825</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.26798679867986797</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.22659279778393362</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.18143459915611823</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.09842154131847723</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.19441210710128046</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.17305751765893052</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.12353766963032291</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.07688869021010278</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1646475770925109</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1420427553444181</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.09477841158402812</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.043589743589743594</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1284722222222223</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.13043478260869557</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.025917926565874723</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.07007822685788775</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.13168086754453925</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.12846260387811642</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.07257304429783208</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.15789473684210534</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.29906542056074764</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.3703703703703703</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1686046511627907</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1370420624151967</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.2837837837837839</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.2978395061728395</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.15691158156911583</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.1138845553822153</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.2630410654827969</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.27223719676549873</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.14465875370919873</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.5275080906148868</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-0.41638225255972694</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.43070787637088737</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-0.39292482627921665</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-0.4794520547945205</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-0.256544502617801</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.27499999999999997</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-0.28571428571428575</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.00873205741626791</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.006404833836857971</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.0040048543689320025</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.006139348943460837</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.029695458979083104</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.03771948840234127</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.030286757598539365</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.06152099886492625</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-0.5579710144927535</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-0.4265734265734265</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.3628318584070796</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-0.38826185101580135</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.022912713472485666</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.01482151705120757</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.013126573474525664</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-0.002070604839458443</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-0.06683804627249353</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.001675041876046833</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.02661596958174902</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0059523809523809165</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-0.5397022332506204</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-0.43162790697674414</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-0.45867287543655416</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-0.4119338605319914</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-0.4117647058823529</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-0.23529411764705882</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-0.09090909090909094</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-0.006659267480577088</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.020114942528735667</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.008720551867759897</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.00466240718356076</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-0.018244013683010363</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.10619803476946339</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.013269819666553299</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.03562054743157109</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-0.008324084350721428</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.20423892100192675</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-0.004162330905307091</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.051546391752577365</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-0.011116051578479334</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.14126394052044614</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.01010101010101011</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.04216600088770532</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0.013682092555331937</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1194274028629857</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-0.012955182072829259</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.03773584905660376</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-0.06532663316582928</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.17408376963350794</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.07011866235167212</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.05412719891745608</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-0.025568980050575996</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.08936525612472149</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-0.021415973796926058</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0329183955739973</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-0.05714285714285713</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.18750000000000006</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-0.05098039215686271</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0724637681159421</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-0.05887681159420283</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.19007490636704105</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-0.06346749226006201</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.06445312499999994</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="n">
+        <v>-0.06032818532818525</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.18089944416371906</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-0.0752458315519453</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.05530973451327439</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.05404404960207293</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.09895470383275275</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.05434782608695648</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.08183800100620485</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="n">
+        <v>-0.07258834765998086</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.1384152457372117</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-0.07749999999999992</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.030769230769230795</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.022936327798351447</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-0.017948096046568076</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.010233566096797438</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-0.008780768677126809</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-0.04729945669542996</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5.042864346948511E-4</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.0368997472620051</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.04019746121297609</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.10671191553544492</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.39526484751203855</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.21423562412342212</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.31622581918673487</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.04205636229387166</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3.9455303539231176E-4</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.013253159896919893</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-0.0032596305124025456</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-0.07441860465116266</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.013245033112582702</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-0.030612244897959176</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.005649717514124259</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.04965883244882487</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.09269863994273456</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.052303429165223424</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.07883888698041899</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-0.2000000000000001</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.1260504201680672</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.22222222222222232</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-0.012001454721784483</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.002022585538513551</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.004055548728032407</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.004809343868086419</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1"/>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="n">
         <v>-0.015846538782318703</v>
       </c>
       <c r="D2" t="n">
@@ -1460,16 +2284,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.12386706948640488</v>
+        <v>-0.05062205062205064</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.09311740890688261</v>
+        <v>-0.031156156156156266</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.11168032786885253</v>
+        <v>-0.01414617716402823</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.11807120324470471</v>
+        <v>0.025995948683322025</v>
       </c>
     </row>
     <row r="3">
@@ -1480,16 +2304,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1378839590443686</v>
+        <v>-0.04161073825503345</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.05607476635514011</v>
+        <v>-0.009248554913294743</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.10044642857142856</v>
+        <v>0.015408320493066126</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.11163416274377945</v>
+        <v>0.061716006021073785</v>
       </c>
     </row>
     <row r="4">
@@ -1500,16 +2324,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.12794033275960995</v>
+        <v>-0.04771677783478709</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.08327501749475154</v>
+        <v>-0.024021352313167207</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.11190903650508674</v>
+        <v>-0.003980891719745226</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.11695906432748535</v>
+        <v>0.040332147093712876</v>
       </c>
     </row>
     <row r="5">
@@ -1520,16 +2344,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1229551451187336</v>
+        <v>-0.04922515952597996</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.08785046728971964</v>
+        <v>-0.027966440271674123</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.11152025249868489</v>
+        <v>-0.012798339674853118</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.11856400566839873</v>
+        <v>0.029287226534933063</v>
       </c>
     </row>
     <row r="6">
@@ -1540,16 +2364,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.24791086350974934</v>
+        <v>-0.10620915032679737</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.1409395973154362</v>
+        <v>-0.07030129124820662</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.17971014492753634</v>
+        <v>-0.025219298245613996</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.22601279317697226</v>
+        <v>0.01795735129068467</v>
       </c>
     </row>
     <row r="7">
@@ -1560,16 +2384,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.120923415170392</v>
+        <v>-0.057411907654920935</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.07603305785123968</v>
+        <v>-0.032538569424964935</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0945945945945947</v>
+        <v>-0.010958904109589078</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.11331351172778327</v>
+        <v>0.014790674354474847</v>
       </c>
     </row>
     <row r="8">
@@ -1580,16 +2404,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.2540983606557377</v>
+        <v>-0.09444444444444446</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.11578947368421055</v>
+        <v>-0.07281553398058259</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.17391304347826086</v>
+        <v>-0.025925925925925897</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.2251655629139073</v>
+        <v>0.03488372093023261</v>
       </c>
     </row>
     <row r="9">
@@ -1600,16 +2424,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.24190800681431013</v>
+        <v>-0.10348837209302317</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.12147505422993493</v>
+        <v>-0.06700507614213207</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.16967509025270755</v>
+        <v>-0.0222222222222222</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.2169680111265647</v>
+        <v>0.027397260273972605</v>
       </c>
     </row>
     <row r="10">
@@ -1620,16 +2444,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.23205506391347094</v>
+        <v>-0.107264086897488</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.13135068153655513</v>
+        <v>-0.06520450503852983</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1671891327063741</v>
+        <v>-0.019514516896715944</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.20734693877551014</v>
+        <v>0.020216267042783256</v>
       </c>
     </row>
     <row r="11">
@@ -1640,16 +2464,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.08017334777898148</v>
+        <v>-0.003205128205128233</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.057191634656423365</v>
+        <v>-0.030062111801242235</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.060800790904597155</v>
+        <v>-0.03102153724560362</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0910458991723099</v>
+        <v>-0.06037567084078705</v>
       </c>
     </row>
     <row r="12">
@@ -1660,16 +2484,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.2712933753943218</v>
+        <v>-0.10619469026548678</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.17589576547231275</v>
+        <v>-0.07525655644241727</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.20312500000000006</v>
+        <v>-0.03015075376884427</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.2505050505050505</v>
+        <v>-0.0034904013961605377</v>
       </c>
     </row>
     <row r="13">
@@ -1680,16 +2504,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.03513022410660209</v>
+        <v>-0.038313685289595126</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.019123020706455465</v>
+        <v>-0.04792746113989641</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.01403808593750008</v>
+        <v>-0.019701419481155166</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.011384925781812808</v>
+        <v>-0.028834894613583212</v>
       </c>
     </row>
     <row r="14">
@@ -1700,16 +2524,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.015508395522388033</v>
+        <v>-0.04044585987261143</v>
       </c>
       <c r="D14" t="n">
-        <v>0.020378632581695304</v>
+        <v>-0.03336791147994465</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.0017736786094360373</v>
+        <v>-0.020723504817306084</v>
       </c>
       <c r="F14" t="n">
-        <v>0.032736177342441004</v>
+        <v>0.02327746741154554</v>
       </c>
     </row>
     <row r="15">
@@ -1720,16 +2544,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.188715953307393</v>
+        <v>0.1138952164009111</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.10402684563758384</v>
+        <v>0.18924581005586602</v>
       </c>
       <c r="E15" t="n">
-        <v>0.019438444924406006</v>
+        <v>0.03293687099725532</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.13351498637602183</v>
+        <v>-0.07419505366308912</v>
       </c>
     </row>
     <row r="16">
@@ -1740,16 +2564,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.07682308232704019</v>
+        <v>0.05941500087673148</v>
       </c>
       <c r="D16" t="n">
-        <v>0.030466301953524833</v>
+        <v>0.020290166997661816</v>
       </c>
       <c r="E16" t="n">
-        <v>0.022615272949535734</v>
+        <v>0.028734211122787328</v>
       </c>
       <c r="F16" t="n">
-        <v>0.018483885610531072</v>
+        <v>-0.022714879694635707</v>
       </c>
     </row>
     <row r="17">
@@ -1760,16 +2584,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.182089552238806</v>
+        <v>-0.12589928057553956</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.06989247311827958</v>
+        <v>-0.07692307692307705</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.03952569169960478</v>
+        <v>-0.052924791086350946</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.044303797468354486</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18">
@@ -1780,16 +2604,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.056547619047619097</v>
+        <v>-0.015067805123053755</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.03595812471552125</v>
+        <v>-0.04591688462656215</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.03638368246968023</v>
+        <v>-0.04006063230835851</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.06636060100166943</v>
+        <v>-0.06663196251952111</v>
       </c>
     </row>
     <row r="19">
@@ -1800,16 +2624,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.41379310344827586</v>
+        <v>-0.2000000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.2000000000000001</v>
+        <v>-0.06451612903225809</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.11111111111111105</v>
+        <v>-0.18750000000000008</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.2222222222222222</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="20">
@@ -1820,16 +2644,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.02832574607991904</v>
+        <v>-0.025724683147195473</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.0482013113592061</v>
+        <v>-0.03677793324005591</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.010800842992623795</v>
+        <v>-0.010642341315089272</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.025187566988210078</v>
+        <v>0.04120824164832957</v>
       </c>
     </row>
   </sheetData>
@@ -1871,16 +2695,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02087332053742799</v>
+        <v>-0.22268907563025206</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.022929936305732503</v>
+        <v>-0.1268260292164675</v>
       </c>
       <c r="E2" t="n">
-        <v>0.013556388808768336</v>
+        <v>-0.057645631067961216</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.06412175648702595</v>
+        <v>-0.28811121764141906</v>
       </c>
     </row>
     <row r="3">
@@ -1891,16 +2715,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>0.06816030293467973</v>
+        <v>-0.2547085201793723</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0485232067510549</v>
+        <v>-0.10728476821192048</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08266414737836555</v>
+        <v>0.03111111111111108</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.04821638573108587</v>
+        <v>-0.32409739714525604</v>
       </c>
     </row>
     <row r="4">
@@ -1911,16 +2735,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>0.04176771759633526</v>
+        <v>-0.23458540042523035</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0015455950540958282</v>
+        <v>-0.11830742659758207</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03672612801678912</v>
+        <v>-0.02841781874039945</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.059173357121617524</v>
+        <v>-0.30232558139534876</v>
       </c>
     </row>
     <row r="5">
@@ -1931,16 +2755,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>0.028028028028027997</v>
+        <v>-0.22539682539682543</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.01590348231423095</v>
+        <v>-0.12243401759530786</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01668653158522048</v>
+        <v>-0.05296343001261029</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.06338397066526978</v>
+        <v>-0.292197858235594</v>
       </c>
     </row>
     <row r="6">
@@ -1951,16 +2775,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.01378070701018572</v>
+        <v>-0.32423208191126274</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.06324110671936757</v>
+        <v>-0.13513513513513511</v>
       </c>
       <c r="E6" t="n">
-        <v>0.010928961748633977</v>
+        <v>-0.019543973941368184</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.14440639269406386</v>
+        <v>-0.4437229437229437</v>
       </c>
     </row>
     <row r="7">
@@ -1971,16 +2795,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00509554140127393</v>
+        <v>-0.1961038961038961</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.02058590657165472</v>
+        <v>-0.0957297043641483</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0071820870299958055</v>
+        <v>-0.033949290932531115</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.06416217221498972</v>
+        <v>-0.2613833854709768</v>
       </c>
     </row>
     <row r="8">
@@ -1991,16 +2815,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.005050505050505078</v>
+        <v>-0.3295454545454546</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0675675675675675</v>
+        <v>-0.1447368421052632</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.009592326139088671</v>
+        <v>-0.044943820224719024</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.16859504132231407</v>
+        <v>-0.4318181818181818</v>
       </c>
     </row>
     <row r="9">
@@ -2011,16 +2835,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0032258064516128837</v>
+        <v>-0.3130841121495327</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.05346350534635058</v>
+        <v>-0.13043478260869562</v>
       </c>
       <c r="E9" t="n">
-        <v>0.005485463521667586</v>
+        <v>-0.02272727272727275</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.13836734693877545</v>
+        <v>-0.4303405572755418</v>
       </c>
     </row>
     <row r="10">
@@ -2031,16 +2855,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0031914893617020716</v>
+        <v>-0.29255319148936176</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.03899721448467967</v>
+        <v>-0.1149068322981366</v>
       </c>
       <c r="E10" t="n">
-        <v>0.015576323987538955</v>
+        <v>0.006345177664974625</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.11524774158226123</v>
+        <v>-0.4232804232804233</v>
       </c>
     </row>
     <row r="11">
@@ -2051,16 +2875,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0818595250126326</v>
+        <v>-0.1515723270440252</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.06432160804020096</v>
+        <v>-0.08507386653082014</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0032644178454842247</v>
+        <v>-0.0458874458874458</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0788203753351207</v>
+        <v>-0.1660377358490565</v>
       </c>
     </row>
     <row r="12">
@@ -2071,16 +2895,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.05613648871766641</v>
+        <v>-0.3485714285714286</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.0762112139357649</v>
+        <v>-0.155223880597015</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01731879409878114</v>
+        <v>-0.018229166666666647</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.14517625231910955</v>
+        <v>-0.4661157024793388</v>
       </c>
     </row>
     <row r="13">
@@ -2091,16 +2915,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>3.2615786040452057E-4</v>
+        <v>-0.028820210939416193</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.006402927052366852</v>
+        <v>-0.024024390243902367</v>
       </c>
       <c r="E13" t="n">
-        <v>9.2571164082391E-4</v>
+        <v>-0.009549461312438686</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.006843800322061183</v>
+        <v>-0.012416979497545395</v>
       </c>
     </row>
     <row r="14">
@@ -2111,16 +2935,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>0.03306981405188726</v>
+        <v>0.0452240646841168</v>
       </c>
       <c r="D14" t="n">
-        <v>0.012870298457783263</v>
+        <v>0.03366906474820157</v>
       </c>
       <c r="E14" t="n">
-        <v>0.011941669537260264</v>
+        <v>0.02627422828427851</v>
       </c>
       <c r="F14" t="n">
-        <v>0.03525681674064686</v>
+        <v>0.0788629069234296</v>
       </c>
     </row>
     <row r="15">
@@ -2131,16 +2955,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.07627475769068691</v>
+        <v>-0.14483394833948332</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.007805724197744996</v>
+        <v>0.10987261146496821</v>
       </c>
       <c r="E15" t="n">
-        <v>0.17987360233349542</v>
+        <v>0.0957642725598526</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.033112582781456984</v>
+        <v>-0.12362204724409454</v>
       </c>
     </row>
     <row r="16">
@@ -2151,16 +2975,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.04716906469126423</v>
+        <v>0.042091301354913374</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.02479854727045745</v>
+        <v>0.00973901113178328</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.05381225797836825</v>
+        <v>-0.017420116464787687</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.011869074354466611</v>
+        <v>0.0016939840673932144</v>
       </c>
     </row>
     <row r="17">
@@ -2171,16 +2995,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>0.041297935103244796</v>
+        <v>-0.09226190476190473</v>
       </c>
       <c r="D17" t="n">
-        <v>0.040522875816993535</v>
+        <v>-0.0017953321364452938</v>
       </c>
       <c r="E17" t="n">
-        <v>0.11455847255369925</v>
+        <v>0.1010452961672475</v>
       </c>
       <c r="F17" t="n">
-        <v>0.043902439024390144</v>
+        <v>0.01257861635220118</v>
       </c>
     </row>
     <row r="18">
@@ -2191,16 +3015,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.06781166716020129</v>
+        <v>-0.15659881812212728</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.052389705882352915</v>
+        <v>-0.09379093528949436</v>
       </c>
       <c r="E18" t="n">
-        <v>0.028726708074534157</v>
+        <v>-0.03988868274582567</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.06592039800995024</v>
+        <v>-0.15137956748695006</v>
       </c>
     </row>
     <row r="19">
@@ -2211,16 +3035,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.09803921568627459</v>
+        <v>-0.29629629629629634</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6842105263157896</v>
+        <v>0.233009708737864</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2173913043478261</v>
+        <v>0.5833333333333335</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8947368421052632</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="20">
@@ -2231,16 +3055,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>0.011221802358868695</v>
+        <v>-0.013063685466650014</v>
       </c>
       <c r="D20" t="n">
-        <v>0.020729426433915354</v>
+        <v>-0.0179442508710801</v>
       </c>
       <c r="E20" t="n">
-        <v>0.01705426356589145</v>
+        <v>0.007094943240454011</v>
       </c>
       <c r="F20" t="n">
-        <v>0.01093329107906832</v>
+        <v>-0.005648720211826974</v>
       </c>
     </row>
   </sheetData>
@@ -2282,16 +3106,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0031914893617021136</v>
+        <v>-0.12386706948640488</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.01486417221937475</v>
+        <v>-0.09311740890688261</v>
       </c>
       <c r="E2" t="n">
-        <v>0.009522272433828123</v>
+        <v>-0.11168032786885253</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.009795782832475354</v>
+        <v>-0.11807120324470471</v>
       </c>
     </row>
     <row r="3">
@@ -2302,16 +3126,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>0.014116749332315838</v>
+        <v>-0.1378839590443686</v>
       </c>
       <c r="D3" t="n">
-        <v>0.030082987551867217</v>
+        <v>-0.05607476635514011</v>
       </c>
       <c r="E3" t="n">
-        <v>0.022332506203473865</v>
+        <v>-0.10044642857142856</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.010692588092344982</v>
+        <v>-0.11163416274377945</v>
       </c>
     </row>
     <row r="4">
@@ -2322,16 +3146,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00750876022025688</v>
+        <v>-0.12794033275960995</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0016207455429498034</v>
+        <v>-0.08327501749475154</v>
       </c>
       <c r="E4" t="n">
-        <v>0.012965363956288212</v>
+        <v>-0.11190903650508674</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.009304128707113833</v>
+        <v>-0.11695906432748535</v>
       </c>
     </row>
     <row r="5">
@@ -2342,16 +3166,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>0.005844258410993582</v>
+        <v>-0.1229551451187336</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.009149130832570913</v>
+        <v>-0.08785046728971964</v>
       </c>
       <c r="E5" t="n">
-        <v>0.010246240290860988</v>
+        <v>-0.11152025249868489</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.009717161200763576</v>
+        <v>-0.11856400566839873</v>
       </c>
     </row>
     <row r="6">
@@ -2362,16 +3186,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>0.013321084060633835</v>
+        <v>-0.24791086350974934</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.06153846153846144</v>
+        <v>-0.1409395973154362</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.012039312039311943</v>
+        <v>-0.17971014492753634</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.03749062734316424</v>
+        <v>-0.22601279317697226</v>
       </c>
     </row>
     <row r="7">
@@ -2382,16 +3206,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>0.003921568627451093</v>
+        <v>-0.120923415170392</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.023020625415834974</v>
+        <v>-0.07603305785123968</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0052083333333333235</v>
+        <v>-0.0945945945945947</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.014743589743589827</v>
+        <v>-0.11331351172778327</v>
       </c>
     </row>
     <row r="8">
@@ -2402,16 +3226,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.038507821901323645</v>
+        <v>-0.2540983606557377</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.13186813186813198</v>
+        <v>-0.11578947368421055</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.10053619302949052</v>
+        <v>-0.17391304347826086</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.1352564102564103</v>
+        <v>-0.2251655629139073</v>
       </c>
     </row>
     <row r="9">
@@ -2422,16 +3246,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>0.004458161865569162</v>
+        <v>-0.24190800681431013</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.06700610997963337</v>
+        <v>-0.12147505422993493</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.021823562049195343</v>
+        <v>-0.16967509025270755</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.0450584090487669</v>
+        <v>-0.2169680111265647</v>
       </c>
     </row>
     <row r="10">
@@ -2442,16 +3266,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>0.003792667509481672</v>
+        <v>-0.23205506391347094</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.04594832648267762</v>
+        <v>-0.13135068153655513</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.007705593197821213</v>
+        <v>-0.1671891327063741</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.028708133971291804</v>
+        <v>-0.20734693877551014</v>
       </c>
     </row>
     <row r="11">
@@ -2462,16 +3286,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0.020806451612903263</v>
+        <v>-0.08017334777898148</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.029113509977101795</v>
+        <v>-0.057191634656423365</v>
       </c>
       <c r="E11" t="n">
-        <v>0.033467974610502015</v>
+        <v>-0.060800790904597155</v>
       </c>
       <c r="F11" t="n">
-        <v>0.012632496006969713</v>
+        <v>-0.0910458991723099</v>
       </c>
     </row>
     <row r="12">
@@ -2482,16 +3306,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>0.020162128455622503</v>
+        <v>-0.2712933753943218</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.04808877928483358</v>
+        <v>-0.17589576547231275</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0019153011278995784</v>
+        <v>-0.20312500000000006</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.02510368915084045</v>
+        <v>-0.2505050505050505</v>
       </c>
     </row>
     <row r="13">
@@ -2502,16 +3326,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.0035846072746441313</v>
+        <v>-0.03513022410660209</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.01270662318677609</v>
+        <v>-0.019123020706455465</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.007689698066267136</v>
+        <v>-0.01403808593750008</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.009146739840585399</v>
+        <v>-0.011384925781812808</v>
       </c>
     </row>
     <row r="14">
@@ -2522,16 +3346,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>0.006069485140226065</v>
+        <v>-0.015508395522388033</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.0011800042909246833</v>
+        <v>0.020378632581695304</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.025873362445414907</v>
+        <v>-0.0017736786094360373</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.0072940332416596846</v>
+        <v>0.032736177342441004</v>
       </c>
     </row>
     <row r="15">
@@ -2542,16 +3366,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.060171256653552475</v>
+        <v>-0.188715953307393</v>
       </c>
       <c r="D15" t="n">
-        <v>0.042244835029294006</v>
+        <v>-0.10402684563758384</v>
       </c>
       <c r="E15" t="n">
-        <v>0.14637514384349826</v>
+        <v>0.019438444924406006</v>
       </c>
       <c r="F15" t="n">
-        <v>0.09820298658567451</v>
+        <v>-0.13351498637602183</v>
       </c>
     </row>
     <row r="16">
@@ -2562,16 +3386,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.040076313263577065</v>
+        <v>0.07682308232704019</v>
       </c>
       <c r="D16" t="n">
-        <v>0.028759493670886056</v>
+        <v>0.030466301953524833</v>
       </c>
       <c r="E16" t="n">
-        <v>0.006846403740474328</v>
+        <v>0.022615272949535734</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.019219685213921624</v>
+        <v>0.018483885610531072</v>
       </c>
     </row>
     <row r="17">
@@ -2582,16 +3406,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>0.009554140127388514</v>
+        <v>-0.182089552238806</v>
       </c>
       <c r="D17" t="n">
-        <v>0.015401540154015386</v>
+        <v>-0.06989247311827958</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.03993344425956738</v>
+        <v>-0.03952569169960478</v>
       </c>
       <c r="F17" t="n">
-        <v>0.015624999999999905</v>
+        <v>-0.044303797468354486</v>
       </c>
     </row>
     <row r="18">
@@ -2602,16 +3426,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>0.03939514524472727</v>
+        <v>-0.056547619047619097</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.022899159663865475</v>
+        <v>-0.03595812471552125</v>
       </c>
       <c r="E18" t="n">
-        <v>0.0463900134952766</v>
+        <v>-0.03638368246968023</v>
       </c>
       <c r="F18" t="n">
-        <v>0.037805521364515496</v>
+        <v>-0.06636060100166943</v>
       </c>
     </row>
     <row r="19">
@@ -2622,16 +3446,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2</v>
+        <v>-0.41379310344827586</v>
       </c>
       <c r="D19" t="n">
-        <v>0.31617647058823534</v>
+        <v>-0.2000000000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0</v>
+        <v>-0.11111111111111105</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9374999999999999</v>
+        <v>-0.2222222222222222</v>
       </c>
     </row>
     <row r="20">
@@ -2642,16 +3466,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0056848653866780775</v>
+        <v>-0.02832574607991904</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.022071307300509265</v>
+        <v>-0.0482013113592061</v>
       </c>
       <c r="E20" t="n">
-        <v>-1.1268875366237208E-4</v>
+        <v>-0.010800842992623795</v>
       </c>
       <c r="F20" t="n">
-        <v>0.011982248520710052</v>
+        <v>-0.025187566988210078</v>
       </c>
     </row>
   </sheetData>
@@ -2693,16 +3517,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.2439189189189189</v>
+        <v>0.02087332053742799</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1793760831889081</v>
+        <v>-0.022929936305732503</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.10170870626525629</v>
+        <v>0.013556388808768336</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0073637702503681944</v>
+        <v>-0.06412175648702595</v>
       </c>
     </row>
     <row r="3">
@@ -2713,16 +3537,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.39793814432989694</v>
+        <v>0.06816030293467973</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1637239165329052</v>
+        <v>0.0485232067510549</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.21109607577807846</v>
+        <v>0.08266414737836555</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.0816542948038176</v>
+        <v>-0.04821638573108587</v>
       </c>
     </row>
     <row r="4">
@@ -2733,16 +3557,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.29976019184652275</v>
+        <v>0.04176771759633526</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1789242590559824</v>
+        <v>-0.0015455950540958282</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.14042126379137412</v>
+        <v>0.03672612801678912</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.02403433476394859</v>
+        <v>-0.059173357121617524</v>
       </c>
     </row>
     <row r="5">
@@ -2753,16 +3577,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.2609006433166547</v>
+        <v>0.028028028028027997</v>
       </c>
       <c r="D5" t="n">
-        <v>0.17580340264650274</v>
+        <v>-0.01590348231423095</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.10792580101180432</v>
+        <v>0.01668653158522048</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.0015420200462606453</v>
+        <v>-0.06338397066526978</v>
       </c>
     </row>
     <row r="6">
@@ -2773,16 +3597,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.3644444444444444</v>
+        <v>-0.01378070701018572</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5037037037037037</v>
+        <v>-0.06324110671936757</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.17610062893081763</v>
+        <v>0.010928961748633977</v>
       </c>
       <c r="F6" t="n">
-        <v>0.058823529411764684</v>
+        <v>-0.14440639269406386</v>
       </c>
     </row>
     <row r="7">
@@ -2793,16 +3617,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.21648460774577954</v>
+        <v>0.00509554140127393</v>
       </c>
       <c r="D7" t="n">
-        <v>0.19148936170212777</v>
+        <v>-0.02058590657165472</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1007615700058582</v>
+        <v>0.0071820870299958055</v>
       </c>
       <c r="F7" t="n">
-        <v>0.009292720702116654</v>
+        <v>-0.06416217221498972</v>
       </c>
     </row>
     <row r="8">
@@ -2813,16 +3637,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.36507936507936506</v>
+        <v>-0.005050505050505078</v>
       </c>
       <c r="D8" t="n">
-        <v>0.44999999999999984</v>
+        <v>-0.0675675675675675</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.17777777777777767</v>
+        <v>-0.009592326139088671</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01639344262295072</v>
+        <v>-0.16859504132231407</v>
       </c>
     </row>
     <row r="9">
@@ -2833,16 +3657,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.3682539682539682</v>
+        <v>0.0032258064516128837</v>
       </c>
       <c r="D9" t="n">
-        <v>0.44162436548223366</v>
+        <v>-0.05346350534635058</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.19026548672566365</v>
+        <v>0.005485463521667586</v>
       </c>
       <c r="F9" t="n">
-        <v>0.009740259740259681</v>
+        <v>-0.13836734693877545</v>
       </c>
     </row>
     <row r="10">
@@ -2853,16 +3677,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.36684303350970016</v>
+        <v>0.0031914893617020716</v>
       </c>
       <c r="D10" t="n">
-        <v>0.43589743589743596</v>
+        <v>-0.03899721448467967</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.19354838709677422</v>
+        <v>0.015576323987538955</v>
       </c>
       <c r="F10" t="n">
-        <v>0.008992805755395692</v>
+        <v>-0.11524774158226123</v>
       </c>
     </row>
     <row r="11">
@@ -2873,16 +3697,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0.1652626362735381</v>
+        <v>-0.0818595250126326</v>
       </c>
       <c r="D11" t="n">
-        <v>0.40766666666666673</v>
+        <v>-0.06432160804020096</v>
       </c>
       <c r="E11" t="n">
-        <v>0.24157764995891537</v>
+        <v>0.0032644178454842247</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3283828382838284</v>
+        <v>-0.0788203753351207</v>
       </c>
     </row>
     <row r="12">
@@ -2893,16 +3717,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.34448160535117056</v>
+        <v>-0.05613648871766641</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6728395061728395</v>
+        <v>-0.0762112139357649</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.1310679611650486</v>
+        <v>0.01731879409878114</v>
       </c>
       <c r="F12" t="n">
-        <v>0.19196428571428578</v>
+        <v>-0.14517625231910955</v>
       </c>
     </row>
     <row r="13">
@@ -2913,16 +3737,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.043707796193983996</v>
+        <v>3.2615786040452057E-4</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.03238916256157648</v>
+        <v>-0.006402927052366852</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.02096793855906375</v>
+        <v>9.2571164082391E-4</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.014035087719298322</v>
+        <v>-0.006843800322061183</v>
       </c>
     </row>
     <row r="14">
@@ -2933,16 +3757,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.14308847342852946</v>
+        <v>0.03306981405188726</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.13410067951740398</v>
+        <v>0.012870298457783263</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.14885100074128974</v>
+        <v>0.011941669537260264</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.08119601328903646</v>
+        <v>0.03525681674064686</v>
       </c>
     </row>
     <row r="15">
@@ -2953,16 +3777,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.42857142857142855</v>
+        <v>-0.07627475769068691</v>
       </c>
       <c r="D15" t="n">
-        <v>1.2848751835535976</v>
+        <v>-0.007805724197744996</v>
       </c>
       <c r="E15" t="n">
-        <v>0.7906976744186045</v>
+        <v>0.17987360233349542</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6989079563182525</v>
+        <v>-0.033112582781456984</v>
       </c>
     </row>
     <row r="16">
@@ -2973,16 +3797,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.08952128443069678</v>
+        <v>-0.04716906469126423</v>
       </c>
       <c r="D16" t="n">
-        <v>0.011766071912373808</v>
+        <v>-0.02479854727045745</v>
       </c>
       <c r="E16" t="n">
-        <v>0.02028682068117373</v>
+        <v>-0.05381225797836825</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.014191855109241768</v>
+        <v>-0.011869074354466611</v>
       </c>
     </row>
     <row r="17">
@@ -2993,16 +3817,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.15217391304347822</v>
+        <v>0.041297935103244796</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0</v>
+        <v>0.040522875816993535</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.03246753246753249</v>
+        <v>0.11455847255369925</v>
       </c>
       <c r="F17" t="n">
-        <v>0.00628930817610059</v>
+        <v>0.043902439024390144</v>
       </c>
     </row>
     <row r="18">
@@ -3013,16 +3837,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>0.1527254458678723</v>
+        <v>-0.06781166716020129</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3862938970337539</v>
+        <v>-0.052389705882352915</v>
       </c>
       <c r="E18" t="n">
-        <v>0.23596442468037793</v>
+        <v>0.028726708074534157</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3227603943420488</v>
+        <v>-0.06592039800995024</v>
       </c>
     </row>
     <row r="19">
@@ -3033,16 +3857,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2</v>
+        <v>-0.09803921568627459</v>
       </c>
       <c r="D19" t="n">
-        <v>0.3661971830985915</v>
+        <v>0.6842105263157896</v>
       </c>
       <c r="E19" t="n">
-        <v>0.16666666666666677</v>
+        <v>0.2173913043478261</v>
       </c>
       <c r="F19" t="n">
-        <v>1.2727272727272727</v>
+        <v>0.8947368421052632</v>
       </c>
     </row>
     <row r="20">
@@ -3053,16 +3877,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.031602155805977514</v>
+        <v>0.011221802358868695</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.021288949100058078</v>
+        <v>0.020729426433915354</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.008671257332313222</v>
+        <v>0.01705426356589145</v>
       </c>
       <c r="F20" t="n">
-        <v>0.02426242236024836</v>
+        <v>0.01093329107906832</v>
       </c>
     </row>
   </sheetData>
@@ -3104,16 +3928,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.0630372492836676</v>
+        <v>0.0031914893617021136</v>
       </c>
       <c r="D2" t="n">
-        <v>0.041751944330740955</v>
+        <v>-0.01486417221937475</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.02828989192625545</v>
+        <v>0.009522272433828123</v>
       </c>
       <c r="F2" t="n">
-        <v>0.06989779096604021</v>
+        <v>-0.009795782832475354</v>
       </c>
     </row>
     <row r="3">
@@ -3124,16 +3948,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0725933719095212</v>
+        <v>0.014116749332315838</v>
       </c>
       <c r="D3" t="n">
-        <v>0.033609352167559614</v>
+        <v>0.030082987551867217</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.047235023041474776</v>
+        <v>0.022332506203473865</v>
       </c>
       <c r="F3" t="n">
-        <v>0.03525523319867792</v>
+        <v>-0.010692588092344982</v>
       </c>
     </row>
     <row r="4">
@@ -3144,16 +3968,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.06706204379562052</v>
+        <v>0.00750876022025688</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03883495145631069</v>
+        <v>0.0016207455429498034</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.03721571330117172</v>
+        <v>0.012965363956288212</v>
       </c>
       <c r="F4" t="n">
-        <v>0.05463347164591971</v>
+        <v>-0.009304128707113833</v>
       </c>
     </row>
     <row r="5">
@@ -3164,16 +3988,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.0701606086221471</v>
+        <v>0.005844258410993582</v>
       </c>
       <c r="D5" t="n">
-        <v>0.038299663299663285</v>
+        <v>-0.009149130832570913</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.02997099581050606</v>
+        <v>0.010246240290860988</v>
       </c>
       <c r="F5" t="n">
-        <v>0.06423553027768483</v>
+        <v>-0.009717161200763576</v>
       </c>
     </row>
     <row r="6">
@@ -3184,16 +4008,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.04267161410018559</v>
+        <v>0.013321084060633835</v>
       </c>
       <c r="D6" t="n">
-        <v>0.05987055016181233</v>
+        <v>-0.06153846153846144</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.013771186440677919</v>
+        <v>-0.012039312039311943</v>
       </c>
       <c r="F6" t="n">
-        <v>0.21515892420537902</v>
+        <v>-0.03749062734316424</v>
       </c>
     </row>
     <row r="7">
@@ -3204,16 +4028,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.05942376950780307</v>
+        <v>0.003921568627451093</v>
       </c>
       <c r="D7" t="n">
-        <v>0.019499417927823</v>
+        <v>-0.023020625415834974</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.022898961284230374</v>
+        <v>-0.0052083333333333235</v>
       </c>
       <c r="F7" t="n">
-        <v>0.06167400881057269</v>
+        <v>-0.014743589743589827</v>
       </c>
     </row>
     <row r="8">
@@ -3224,16 +4048,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.15300546448087435</v>
+        <v>-0.038507821901323645</v>
       </c>
       <c r="D8" t="n">
-        <v>0.025773195876288683</v>
+        <v>-0.13186813186813198</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.03793103448275863</v>
+        <v>-0.10053619302949052</v>
       </c>
       <c r="F8" t="n">
-        <v>0.12546125461254615</v>
+        <v>-0.1352564102564103</v>
       </c>
     </row>
     <row r="9">
@@ -3244,16 +4068,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.1152073732718895</v>
+        <v>0.004458161865569162</v>
       </c>
       <c r="D9" t="n">
-        <v>0.021298174442190718</v>
+        <v>-0.06700610997963337</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.04664310954063601</v>
+        <v>-0.021823562049195343</v>
       </c>
       <c r="F9" t="n">
-        <v>0.12720588235294103</v>
+        <v>-0.0450584090487669</v>
       </c>
     </row>
     <row r="10">
@@ -3264,16 +4088,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.08175675675675675</v>
+        <v>0.003792667509481672</v>
       </c>
       <c r="D10" t="n">
-        <v>0.011647254575707259</v>
+        <v>-0.04594832648267762</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.05378973105134481</v>
+        <v>-0.007705593197821213</v>
       </c>
       <c r="F10" t="n">
-        <v>0.12186084808563201</v>
+        <v>-0.028708133971291804</v>
       </c>
     </row>
     <row r="11">
@@ -3284,16 +4108,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0.3161693936477382</v>
+        <v>0.020806451612903263</v>
       </c>
       <c r="D11" t="n">
-        <v>0.24127906976744193</v>
+        <v>-0.029113509977101795</v>
       </c>
       <c r="E11" t="n">
-        <v>0.22485422740524796</v>
+        <v>0.033467974610502015</v>
       </c>
       <c r="F11" t="n">
-        <v>0.45116279069767456</v>
+        <v>0.012632496006969713</v>
       </c>
     </row>
     <row r="12">
@@ -3304,16 +4128,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>0.16666666666666663</v>
+        <v>0.020162128455622503</v>
       </c>
       <c r="D12" t="n">
-        <v>0.17721518987341778</v>
+        <v>-0.04808877928483358</v>
       </c>
       <c r="E12" t="n">
-        <v>0.08316633266533068</v>
+        <v>0.0019153011278995784</v>
       </c>
       <c r="F12" t="n">
-        <v>0.4921383647798741</v>
+        <v>-0.02510368915084045</v>
       </c>
     </row>
     <row r="13">
@@ -3324,16 +4148,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>0.036728563626433536</v>
+        <v>-0.0035846072746441313</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.02260317460317451</v>
+        <v>-0.01270662318677609</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0012208521548040543</v>
+        <v>-0.007689698066267136</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.002864919066036387</v>
+        <v>-0.009146739840585399</v>
       </c>
     </row>
     <row r="14">
@@ -3344,16 +4168,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.013667117726657643</v>
+        <v>0.006069485140226065</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.007851797325481625</v>
+        <v>-0.0011800042909246833</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.007304983042003573</v>
+        <v>-0.025873362445414907</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.019829059829059796</v>
+        <v>-0.0072940332416596846</v>
       </c>
     </row>
     <row r="15">
@@ -3364,16 +4188,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5373711340206185</v>
+        <v>0.060171256653552475</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6246458923512749</v>
+        <v>0.042244835029294006</v>
       </c>
       <c r="E15" t="n">
-        <v>0.29635145197319435</v>
+        <v>0.14637514384349826</v>
       </c>
       <c r="F15" t="n">
-        <v>0.6837146702557197</v>
+        <v>0.09820298658567451</v>
       </c>
     </row>
     <row r="16">
@@ -3384,16 +4208,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.09566849552411205</v>
+        <v>-0.040076313263577065</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.05856860434541258</v>
+        <v>0.028759493670886056</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.06714445688689816</v>
+        <v>0.006846403740474328</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.09791099182823271</v>
+        <v>-0.019219685213921624</v>
       </c>
     </row>
     <row r="17">
@@ -3404,16 +4228,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>0.41064638783269963</v>
+        <v>0.009554140127388514</v>
       </c>
       <c r="D17" t="n">
-        <v>0.19811320754716985</v>
+        <v>0.015401540154015386</v>
       </c>
       <c r="E17" t="n">
-        <v>0.019880715705765425</v>
+        <v>-0.03993344425956738</v>
       </c>
       <c r="F17" t="n">
-        <v>0.12451361867704272</v>
+        <v>0.015624999999999905</v>
       </c>
     </row>
     <row r="18">
@@ -3424,16 +4248,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>0.3658675799086759</v>
+        <v>0.03939514524472727</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2915407854984896</v>
+        <v>-0.022899159663865475</v>
       </c>
       <c r="E18" t="n">
-        <v>0.2792718245759205</v>
+        <v>0.0463900134952766</v>
       </c>
       <c r="F18" t="n">
-        <v>0.4772162386081192</v>
+        <v>0.037805521364515496</v>
       </c>
     </row>
     <row r="19">
@@ -3444,16 +4268,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.31617647058823534</v>
+      </c>
+      <c r="E19" t="n">
         <v>0.0</v>
       </c>
-      <c r="D19" t="n">
-        <v>0.09844559585492221</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.14814814814814806</v>
-      </c>
       <c r="F19" t="n">
-        <v>1.9411764705882353</v>
+        <v>0.9374999999999999</v>
       </c>
     </row>
     <row r="20">
@@ -3464,16 +4288,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0484173819742488</v>
+        <v>0.0056848653866780775</v>
       </c>
       <c r="D20" t="n">
-        <v>0.08197029516826465</v>
+        <v>-0.022071307300509265</v>
       </c>
       <c r="E20" t="n">
-        <v>0.0261437908496732</v>
+        <v>-1.1268875366237208E-4</v>
       </c>
       <c r="F20" t="n">
-        <v>0.11039603960396052</v>
+        <v>0.011982248520710052</v>
       </c>
     </row>
   </sheetData>
@@ -3515,16 +4339,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.020481310803891466</v>
+        <v>-0.2439189189189189</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>0.1793760831889081</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.055804823331463756</v>
+        <v>-0.10170870626525629</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.13854835571122795</v>
+        <v>0.0073637702503681944</v>
       </c>
     </row>
     <row r="3">
@@ -3535,16 +4359,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.0473026840287006</v>
+        <v>-0.39793814432989694</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.009154929577464823</v>
+        <v>0.1637239165329052</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.09450679267572365</v>
+        <v>-0.21109607577807846</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.17800081933633763</v>
+        <v>-0.0816542948038176</v>
       </c>
     </row>
     <row r="4">
@@ -3555,16 +4379,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.033315981259760485</v>
+        <v>-0.29976019184652275</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.004124656278643501</v>
+        <v>0.1789242590559824</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.07292563881711163</v>
+        <v>-0.14042126379137412</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.1560509554140127</v>
+        <v>-0.02403433476394859</v>
       </c>
     </row>
     <row r="5">
@@ -3575,16 +4399,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.026532715095311632</v>
+        <v>-0.2609006433166547</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0015865820489573401</v>
+        <v>0.17580340264650274</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.05915492957746469</v>
+        <v>-0.10792580101180432</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.144481474220741</v>
+        <v>-0.0015420200462606453</v>
       </c>
     </row>
     <row r="6">
@@ -3595,16 +4419,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0418794688457609</v>
+        <v>-0.3644444444444444</v>
       </c>
       <c r="D6" t="n">
-        <v>0.021126760563380344</v>
+        <v>0.5037037037037037</v>
       </c>
       <c r="E6" t="n">
-        <v>0.061757719714964326</v>
+        <v>-0.17610062893081763</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.16817532158170556</v>
+        <v>0.058823529411764684</v>
       </c>
     </row>
     <row r="7">
@@ -3615,16 +4439,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.036931277365315006</v>
+        <v>-0.21648460774577954</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.02466598150051382</v>
+        <v>0.19148936170212777</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.04113858300436315</v>
+        <v>-0.1007615700058582</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.1161242603550296</v>
+        <v>0.009292720702116654</v>
       </c>
     </row>
     <row r="8">
@@ -3635,16 +4459,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.36531365313653136</v>
+        <v>-0.36507936507936506</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.3176206509539843</v>
+        <v>0.44999999999999984</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.27009646302250795</v>
+        <v>-0.17777777777777767</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.41935483870967744</v>
+        <v>0.01639344262295072</v>
       </c>
     </row>
     <row r="9">
@@ -3655,16 +4479,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.1219715956558062</v>
+        <v>-0.3682539682539682</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.08207646439845678</v>
+        <v>0.44162436548223366</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.10114030738720874</v>
+        <v>-0.19026548672566365</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.2415902140672784</v>
+        <v>0.009740259740259681</v>
       </c>
     </row>
     <row r="10">
@@ -3675,16 +4499,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.11000552791597568</v>
+        <v>-0.36684303350970016</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.05729653882132827</v>
+        <v>0.43589743589743596</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.07088186356073206</v>
+        <v>-0.19354838709677422</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.19503063308373048</v>
+        <v>0.008992805755395692</v>
       </c>
     </row>
     <row r="11">
@@ -3695,16 +4519,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>1.0831556503198294</v>
+        <v>0.1652626362735381</v>
       </c>
       <c r="D11" t="n">
-        <v>0.4781976744186046</v>
+        <v>0.40766666666666673</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9026548672566371</v>
+        <v>0.24157764995891537</v>
       </c>
       <c r="F11" t="n">
-        <v>0.267524115755627</v>
+        <v>0.3283828382838284</v>
       </c>
     </row>
     <row r="12">
@@ -3715,16 +4539,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7201492537313433</v>
+        <v>-0.34448160535117056</v>
       </c>
       <c r="D12" t="n">
-        <v>0.38262910798122074</v>
+        <v>0.6728395061728395</v>
       </c>
       <c r="E12" t="n">
-        <v>0.7764705882352942</v>
+        <v>-0.1310679611650486</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0651465798045602</v>
+        <v>0.19196428571428578</v>
       </c>
     </row>
     <row r="13">
@@ -3735,16 +4559,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0015628488501897263</v>
+        <v>-0.043707796193983996</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.025214966302579654</v>
+        <v>-0.03238916256157648</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.011958146487294556</v>
+        <v>-0.02096793855906375</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.047625144027653325</v>
+        <v>-0.014035087719298322</v>
       </c>
     </row>
     <row r="14">
@@ -3755,16 +4579,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.010397553516819558</v>
+        <v>-0.14308847342852946</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.007262684124386247</v>
+        <v>-0.13410067951740398</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.01412171086050992</v>
+        <v>-0.14885100074128974</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.030967078189300428</v>
+        <v>-0.08119601328903646</v>
       </c>
     </row>
     <row r="15">
@@ -3775,16 +4599,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>1.5679611650485439</v>
+        <v>0.42857142857142855</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8813056379821957</v>
+        <v>1.2848751835535976</v>
       </c>
       <c r="E15" t="n">
-        <v>1.225941422594142</v>
+        <v>0.7906976744186045</v>
       </c>
       <c r="F15" t="n">
-        <v>0.20491803278688514</v>
+        <v>0.6989079563182525</v>
       </c>
     </row>
     <row r="16">
@@ -3795,16 +4619,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.1060418351779992</v>
+        <v>0.08952128443069678</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.031006067191886227</v>
+        <v>0.011766071912373808</v>
       </c>
       <c r="E16" t="n">
-        <v>0.008581825207702731</v>
+        <v>0.02028682068117373</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.004736736468856521</v>
+        <v>-0.014191855109241768</v>
       </c>
     </row>
     <row r="17">
@@ -3815,16 +4639,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>0.15863141524105756</v>
+        <v>-0.15217391304347822</v>
       </c>
       <c r="D17" t="n">
-        <v>0.100767754318618</v>
+        <v>0.0</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.04718693284936488</v>
+        <v>-0.03246753246753249</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.23408624229979466</v>
+        <v>0.00628930817610059</v>
       </c>
     </row>
     <row r="18">
@@ -3835,16 +4659,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>1.7040816326530615</v>
+        <v>0.1527254458678723</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7046004842615011</v>
+        <v>0.3862938970337539</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9203747072599532</v>
+        <v>0.23596442468037793</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5635018495684339</v>
+        <v>0.3227603943420488</v>
       </c>
     </row>
     <row r="19">
@@ -3855,16 +4679,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2884615384615384</v>
+        <v>-0.2</v>
       </c>
       <c r="D19" t="n">
-        <v>0.9931506849315069</v>
+        <v>0.3661971830985915</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0</v>
+        <v>0.16666666666666677</v>
       </c>
       <c r="F19" t="n">
-        <v>2.666666666666667</v>
+        <v>1.2727272727272727</v>
       </c>
     </row>
     <row r="20">
@@ -3875,16 +4699,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>0.012467476149176013</v>
+        <v>-0.031602155805977514</v>
       </c>
       <c r="D20" t="n">
-        <v>0.010906862745098063</v>
+        <v>-0.021288949100058078</v>
       </c>
       <c r="E20" t="n">
-        <v>6.694934166481198E-4</v>
+        <v>-0.008671257332313222</v>
       </c>
       <c r="F20" t="n">
-        <v>0.011914217633042108</v>
+        <v>0.02426242236024836</v>
       </c>
     </row>
   </sheetData>
@@ -3926,16 +4750,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.04277062831188485</v>
+        <v>-0.0630372492836676</v>
       </c>
       <c r="D2" t="n">
-        <v>0.04782237403928273</v>
+        <v>0.041751944330740955</v>
       </c>
       <c r="E2" t="n">
-        <v>0.07702020202020206</v>
+        <v>-0.02828989192625545</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.014170040485829972</v>
+        <v>0.06989779096604021</v>
       </c>
     </row>
     <row r="3">
@@ -3946,16 +4770,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.028555431131019153</v>
+        <v>-0.0725933719095212</v>
       </c>
       <c r="D3" t="n">
-        <v>0.17752808988764043</v>
+        <v>0.033609352167559614</v>
       </c>
       <c r="E3" t="n">
-        <v>0.16430412371134018</v>
+        <v>-0.047235023041474776</v>
       </c>
       <c r="F3" t="n">
-        <v>0.07799074686054201</v>
+        <v>0.03525523319867792</v>
       </c>
     </row>
     <row r="4">
@@ -3966,16 +4790,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.03434433541480826</v>
+        <v>-0.06706204379562052</v>
       </c>
       <c r="D4" t="n">
-        <v>0.09531416400425985</v>
+        <v>0.03883495145631069</v>
       </c>
       <c r="E4" t="n">
-        <v>0.11016096579476863</v>
+        <v>-0.03721571330117172</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01877470355731224</v>
+        <v>0.05463347164591971</v>
       </c>
     </row>
     <row r="5">
@@ -3986,16 +4810,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.038369304556354795</v>
+        <v>-0.0701606086221471</v>
       </c>
       <c r="D5" t="n">
-        <v>0.06552044609665428</v>
+        <v>0.038299663299663285</v>
       </c>
       <c r="E5" t="n">
-        <v>0.082827406764961</v>
+        <v>-0.02997099581050606</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.004286326618088302</v>
+        <v>0.06423553027768483</v>
       </c>
     </row>
     <row r="6">
@@ -4006,16 +4830,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.0654761904761905</v>
+        <v>-0.04267161410018559</v>
       </c>
       <c r="D6" t="n">
-        <v>0.08803986710963466</v>
+        <v>0.05987055016181233</v>
       </c>
       <c r="E6" t="n">
-        <v>0.12727272727272726</v>
+        <v>-0.013771186440677919</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.08306709265175724</v>
+        <v>0.21515892420537902</v>
       </c>
     </row>
     <row r="7">
@@ -4026,16 +4850,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.024444444444444373</v>
+        <v>-0.05942376950780307</v>
       </c>
       <c r="D7" t="n">
-        <v>0.04838221953432118</v>
+        <v>0.019499417927823</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0749846342962507</v>
+        <v>-0.022898961284230374</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.024992734670154015</v>
+        <v>0.06167400881057269</v>
       </c>
     </row>
     <row r="8">
@@ -4046,16 +4870,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.029411764705882464</v>
+        <v>-0.15300546448087435</v>
       </c>
       <c r="D8" t="n">
-        <v>0.19597989949748745</v>
+        <v>0.025773195876288683</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1902173913043478</v>
+        <v>-0.03793103448275863</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.03755868544600933</v>
+        <v>0.12546125461254615</v>
       </c>
     </row>
     <row r="9">
@@ -4066,16 +4890,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.03380281690140838</v>
+        <v>-0.1152073732718895</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1450549450549451</v>
+        <v>0.021298174442190718</v>
       </c>
       <c r="E9" t="n">
-        <v>0.17273795534665107</v>
+        <v>-0.04664310954063601</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.04428424304840383</v>
+        <v>0.12720588235294103</v>
       </c>
     </row>
     <row r="10">
@@ -4086,16 +4910,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.03859447004608301</v>
+        <v>-0.08175675675675675</v>
       </c>
       <c r="D10" t="n">
-        <v>0.10942649967040213</v>
+        <v>0.011647254575707259</v>
       </c>
       <c r="E10" t="n">
-        <v>0.15400843881856544</v>
+        <v>-0.05378973105134481</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.05400372439478576</v>
+        <v>0.12186084808563201</v>
       </c>
     </row>
     <row r="11">
@@ -4106,16 +4930,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.11863117870722435</v>
+        <v>0.3161693936477382</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.1265619993591797</v>
+        <v>0.24127906976744193</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.125230882896195</v>
+        <v>0.22485422740524796</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.15123010130246012</v>
+        <v>0.45116279069767456</v>
       </c>
     </row>
     <row r="12">
@@ -4126,16 +4950,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.13533834586466167</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.017964071856287317</v>
+        <v>0.17721518987341778</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01929824561403503</v>
+        <v>0.08316633266533068</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.1725731895223421</v>
+        <v>0.4921383647798741</v>
       </c>
     </row>
     <row r="13">
@@ -4146,16 +4970,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.03215011354129322</v>
+        <v>0.036728563626433536</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.023339317773788237</v>
+        <v>-0.02260317460317451</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.01564964212058719</v>
+        <v>0.0012208521548040543</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.020405271361768413</v>
+        <v>-0.002864919066036387</v>
       </c>
     </row>
     <row r="14">
@@ -4166,16 +4990,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>0.004040404040404016</v>
+        <v>-0.013667117726657643</v>
       </c>
       <c r="D14" t="n">
-        <v>0.018035061167864772</v>
+        <v>-0.007851797325481625</v>
       </c>
       <c r="E14" t="n">
-        <v>0.014320419383710507</v>
+        <v>-0.007304983042003573</v>
       </c>
       <c r="F14" t="n">
-        <v>0.02453271028037387</v>
+        <v>-0.019829059829059796</v>
       </c>
     </row>
     <row r="15">
@@ -4186,16 +5010,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.2678571428571429</v>
+        <v>0.5373711340206185</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.25562372188139054</v>
+        <v>0.6246458923512749</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.18825100133511344</v>
+        <v>0.29635145197319435</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.28428927680798</v>
+        <v>0.6837146702557197</v>
       </c>
     </row>
     <row r="16">
@@ -4206,16 +5030,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.07521764544612793</v>
+        <v>-0.09566849552411205</v>
       </c>
       <c r="D16" t="n">
-        <v>0.04479179288339593</v>
+        <v>-0.05856860434541258</v>
       </c>
       <c r="E16" t="n">
-        <v>0.05571431257167572</v>
+        <v>-0.06714445688689816</v>
       </c>
       <c r="F16" t="n">
-        <v>0.051067840345515564</v>
+        <v>-0.09791099182823271</v>
       </c>
     </row>
     <row r="17">
@@ -4226,16 +5050,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.22641509433962267</v>
+        <v>0.41064638783269963</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.11090573012939012</v>
+        <v>0.19811320754716985</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.09505703422053227</v>
+        <v>0.019880715705765425</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.09493670886075957</v>
+        <v>0.12451361867704272</v>
       </c>
     </row>
     <row r="18">
@@ -4246,16 +5070,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.09608540925266908</v>
+        <v>0.3658675799086759</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.11455576559546321</v>
+        <v>0.2915407854984896</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.12208800690250224</v>
+        <v>0.2792718245759205</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.12062937062937068</v>
+        <v>0.4772162386081192</v>
       </c>
     </row>
     <row r="19">
@@ -4266,16 +5090,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.06250000000000003</v>
+        <v>0.0</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.75</v>
+        <v>0.09844559585492221</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.375</v>
+        <v>0.14814814814814806</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.2857142857142857</v>
+        <v>1.9411764705882353</v>
       </c>
     </row>
     <row r="20">
@@ -4286,16 +5110,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.0325277596342259</v>
+        <v>0.0484173819742488</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.07859778597785982</v>
+        <v>0.08197029516826465</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.028306878306878273</v>
+        <v>0.0261437908496732</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.06290555155010803</v>
+        <v>0.11039603960396052</v>
       </c>
     </row>
   </sheetData>
@@ -4337,16 +5161,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.1660839160839161</v>
+        <v>-0.020481310803891466</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.07484076433121019</v>
+        <v>0.0</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.10225140712945598</v>
+        <v>-0.055804823331463756</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.08454312553373179</v>
+        <v>-0.13854835571122795</v>
       </c>
     </row>
     <row r="3">
@@ -4357,16 +5181,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.26457399103139007</v>
+        <v>-0.0473026840287006</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.19405940594059404</v>
+        <v>-0.009154929577464823</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.20720221606648195</v>
+        <v>-0.09450679267572365</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.19778481012658217</v>
+        <v>-0.17800081933633763</v>
       </c>
     </row>
     <row r="4">
@@ -4377,16 +5201,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.20612813370473534</v>
+        <v>-0.033315981259760485</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.12339930151338764</v>
+        <v>-0.004124656278643501</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.14883955600403634</v>
+        <v>-0.07292563881711163</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.13102480112306972</v>
+        <v>-0.1560509554140127</v>
       </c>
     </row>
     <row r="5">
@@ -4397,16 +5221,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1788109074653554</v>
+        <v>-0.026532715095311632</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.09306167400881056</v>
+        <v>-0.0015865820489573401</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.11021377672209026</v>
+        <v>-0.05915492957746469</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.09784993418165856</v>
+        <v>-0.144481474220741</v>
       </c>
     </row>
     <row r="6">
@@ -4417,16 +5241,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.21282051282051279</v>
+        <v>0.0418794688457609</v>
       </c>
       <c r="D6" t="n">
-        <v>0.003472222222222201</v>
+        <v>0.021126760563380344</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.08115942028985518</v>
+        <v>0.061757719714964326</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.08639308855291584</v>
+        <v>-0.16817532158170556</v>
       </c>
     </row>
     <row r="7">
@@ -4437,16 +5261,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.15319426336375502</v>
+        <v>-0.036931277365315006</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.05499612703330748</v>
+        <v>-0.02466598150051382</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.09833795013850409</v>
+        <v>-0.04113858300436315</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.08545397423814012</v>
+        <v>-0.1161242603550296</v>
       </c>
     </row>
     <row r="8">
@@ -4457,16 +5281,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.3026315789473684</v>
+        <v>-0.36531365313653136</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.09345794392523357</v>
+        <v>-0.3176206509539843</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1925925925925926</v>
+        <v>-0.27009646302250795</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.19767441860465118</v>
+        <v>-0.41935483870967744</v>
       </c>
     </row>
     <row r="9">
@@ -4477,16 +5301,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.29579375848032563</v>
+        <v>-0.1219715956558062</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.09845559845559847</v>
+        <v>-0.08207646439845678</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.18518518518518515</v>
+        <v>-0.10114030738720874</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.17808219178082185</v>
+        <v>-0.2415902140672784</v>
       </c>
     </row>
     <row r="10">
@@ -4497,16 +5321,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.2909516380655227</v>
+        <v>-0.11000552791597568</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.09988901220865698</v>
+        <v>-0.05729653882132827</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.17520215633423172</v>
+        <v>-0.07088186356073206</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.16097922848664686</v>
+        <v>-0.19503063308373048</v>
       </c>
     </row>
     <row r="11">
@@ -4517,16 +5341,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6235167206040991</v>
+        <v>1.0831556503198294</v>
       </c>
       <c r="D11" t="n">
-        <v>0.6629692832764504</v>
+        <v>0.4781976744186046</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6819541375872382</v>
+        <v>0.9026548672566371</v>
       </c>
       <c r="F11" t="n">
-        <v>0.4977890082122553</v>
+        <v>0.267524115755627</v>
       </c>
     </row>
     <row r="12">
@@ -4537,16 +5361,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>0.10958904109589039</v>
+        <v>0.7201492537313433</v>
       </c>
       <c r="D12" t="n">
-        <v>0.387434554973822</v>
+        <v>0.38262910798122074</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3299999999999999</v>
+        <v>0.7764705882352942</v>
       </c>
       <c r="F12" t="n">
-        <v>0.20857142857142838</v>
+        <v>0.0651465798045602</v>
       </c>
     </row>
     <row r="13">
@@ -4557,16 +5381,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.030263157894736832</v>
+        <v>0.0015628488501897263</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.018610271903323226</v>
+        <v>-0.025214966302579654</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.014927184466019391</v>
+        <v>-0.011958146487294556</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.014134780125642519</v>
+        <v>-0.047625144027653325</v>
       </c>
     </row>
     <row r="14">
@@ -4577,16 +5401,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.05353852823236155</v>
+        <v>-0.010397553516819558</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.051159765879037526</v>
+        <v>-0.007262684124386247</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.06154011384384064</v>
+        <v>-0.01412171086050992</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.06560726447219065</v>
+        <v>-0.030967078189300428</v>
       </c>
     </row>
     <row r="15">
@@ -4597,16 +5421,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.358695652173913</v>
+        <v>1.5679611650485439</v>
       </c>
       <c r="D15" t="n">
-        <v>0.6573426573426573</v>
+        <v>0.8813056379821957</v>
       </c>
       <c r="E15" t="n">
-        <v>0.933628318584071</v>
+        <v>1.225941422594142</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4650112866817156</v>
+        <v>0.20491803278688514</v>
       </c>
     </row>
     <row r="16">
@@ -4617,16 +5441,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.10646347248576854</v>
+        <v>-0.1060418351779992</v>
       </c>
       <c r="D16" t="n">
-        <v>0.05658243391714615</v>
+        <v>-0.031006067191886227</v>
       </c>
       <c r="E16" t="n">
-        <v>0.03697971258681674</v>
+        <v>0.008581825207702731</v>
       </c>
       <c r="F16" t="n">
-        <v>0.029814852643503083</v>
+        <v>-0.004736736468856521</v>
       </c>
     </row>
     <row r="17">
@@ -4637,16 +5461,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.22107969151670945</v>
+        <v>0.15863141524105756</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.08375209380234513</v>
+        <v>0.100767754318618</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.05323193916349817</v>
+        <v>-0.04718693284936488</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.07142857142857141</v>
+        <v>-0.23408624229979466</v>
       </c>
     </row>
     <row r="18">
@@ -4657,16 +5481,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7270471464019849</v>
+        <v>1.7040816326530615</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7246511627906977</v>
+        <v>0.7046004842615011</v>
       </c>
       <c r="E18" t="n">
-        <v>0.7788125727590219</v>
+        <v>0.9203747072599532</v>
       </c>
       <c r="F18" t="n">
-        <v>0.5629043853342919</v>
+        <v>0.5635018495684339</v>
       </c>
     </row>
     <row r="19">
@@ -4677,16 +5501,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.47058823529411764</v>
+        <v>-0.2884615384615384</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.14705882352941177</v>
+        <v>0.9931506849315069</v>
       </c>
       <c r="E19" t="n">
         <v>0.0</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.18181818181818188</v>
+        <v>2.666666666666667</v>
       </c>
     </row>
     <row r="20">
@@ -4697,16 +5521,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.03440621531631512</v>
+        <v>0.012467476149176013</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.06913455037187297</v>
+        <v>0.010906862745098063</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.017571261226083504</v>
+        <v>6.694934166481198E-4</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.039371438438956886</v>
+        <v>0.011914217633042108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update aesthetics on barcharts
</commit_message>
<xml_diff>
--- a/tables/change_in_segs.xlsx
+++ b/tables/change_in_segs.xlsx
@@ -7,11 +7,11 @@
   </bookViews>
   <sheets>
     <sheet name="Employed" r:id="rId3" sheetId="1"/>
-    <sheet name="Grade 1 or 2" r:id="rId4" sheetId="2"/>
-    <sheet name="Home Owner" r:id="rId5" sheetId="3"/>
-    <sheet name="Inactive" r:id="rId6" sheetId="4"/>
-    <sheet name="LLTI" r:id="rId7" sheetId="5"/>
-    <sheet name="No Car" r:id="rId8" sheetId="6"/>
+    <sheet name="Grades 3 to 5" r:id="rId4" sheetId="2"/>
+    <sheet name="Has Car" r:id="rId5" sheetId="3"/>
+    <sheet name="Home Owner" r:id="rId6" sheetId="4"/>
+    <sheet name="Inactive" r:id="rId7" sheetId="5"/>
+    <sheet name="LLTI" r:id="rId8" sheetId="6"/>
     <sheet name="Non-house" r:id="rId9" sheetId="7"/>
     <sheet name="Non-religious" r:id="rId10" sheetId="8"/>
     <sheet name="Not Scottish" r:id="rId11" sheetId="9"/>
@@ -2816,16 +2816,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.09444444444444446</v>
+        <v>-0.11931818181818188</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.07281553398058259</v>
+        <v>-0.06896551724137924</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.025925925925925897</v>
+        <v>-0.02316602316602316</v>
       </c>
       <c r="F8" t="n">
-        <v>0.03488372093023261</v>
+        <v>0.02290076335877862</v>
       </c>
     </row>
     <row r="9">
@@ -2856,16 +2856,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.107264086897488</v>
+        <v>-0.09006622516556292</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.06520450503852983</v>
+        <v>-0.06389214536928484</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.019514516896715944</v>
+        <v>-0.022435897435897505</v>
       </c>
       <c r="F10" t="n">
-        <v>0.020216267042783256</v>
+        <v>0.030519790176442484</v>
       </c>
     </row>
     <row r="11">
@@ -2876,16 +2876,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.003205128205128233</v>
+        <v>-0.011054024599096988</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.030062111801242235</v>
+        <v>0.008026853473438338</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.03102153724560362</v>
+        <v>0.01972611672644278</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.06037567084078705</v>
+        <v>0.03985615822595139</v>
       </c>
     </row>
     <row r="12">
@@ -2916,16 +2916,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.038313685289595126</v>
+        <v>-0.021523178807947053</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.04792746113989641</v>
+        <v>-0.02505297270347751</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.019701419481155166</v>
+        <v>-0.011617846990483346</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.028834894613583212</v>
+        <v>-0.01025791324736226</v>
       </c>
     </row>
     <row r="14">
@@ -2936,16 +2936,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.04044585987261143</v>
+        <v>0.07799290973547847</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.03336791147994465</v>
+        <v>0.0510913888222595</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.020723504817306084</v>
+        <v>0.026333407721490686</v>
       </c>
       <c r="F14" t="n">
-        <v>0.02327746741154554</v>
+        <v>-0.027879835746704176</v>
       </c>
     </row>
     <row r="15">
@@ -2956,16 +2956,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.1138952164009111</v>
+        <v>0.10100130605137148</v>
       </c>
       <c r="D15" t="n">
-        <v>0.18924581005586602</v>
+        <v>0.15255423372988114</v>
       </c>
       <c r="E15" t="n">
-        <v>0.03293687099725532</v>
+        <v>0.35986653956148723</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.07419505366308912</v>
+        <v>0.28040540540540543</v>
       </c>
     </row>
     <row r="16">
@@ -2976,16 +2976,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.05941500087673148</v>
+        <v>0.021827593353654483</v>
       </c>
       <c r="D16" t="n">
-        <v>0.020290166997661816</v>
+        <v>-0.00782888298615962</v>
       </c>
       <c r="E16" t="n">
-        <v>0.028734211122787328</v>
+        <v>-0.0015085012222495198</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.022714879694635707</v>
+        <v>-0.02590303985402069</v>
       </c>
     </row>
     <row r="17">
@@ -2996,16 +2996,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.12589928057553956</v>
+        <v>-0.040485829959514205</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.07692307692307705</v>
+        <v>0.006276150627614952</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.052924791086350946</v>
+        <v>0.008510638297872289</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0</v>
+        <v>0.03703703703703707</v>
       </c>
     </row>
     <row r="18">
@@ -3016,16 +3016,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.015067805123053755</v>
+        <v>-0.010249839846252341</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.04591688462656215</v>
+        <v>0.008721359940872161</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.04006063230835851</v>
+        <v>0.015972812234494416</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.06663196251952111</v>
+        <v>0.035277947464874615</v>
       </c>
     </row>
     <row r="19">
@@ -3036,16 +3036,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2000000000000001</v>
+        <v>-0.2173913043478261</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.06451612903225809</v>
+        <v>0.11538461538461536</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.18750000000000008</v>
+        <v>-0.09090909090909094</v>
       </c>
       <c r="F19" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.5000000000000001</v>
       </c>
     </row>
     <row r="20">
@@ -3056,16 +3056,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.025724683147195473</v>
+        <v>-0.01185822256971592</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.03677793324005591</v>
+        <v>0.01580611169652267</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.010642341315089272</v>
+        <v>0.0013517166801838346</v>
       </c>
       <c r="F20" t="n">
-        <v>0.04120824164832957</v>
+        <v>0.04926108374384229</v>
       </c>
     </row>
   </sheetData>
@@ -3107,16 +3107,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.041371158392434895</v>
+        <v>0.02087332053742799</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.003875968992247994</v>
+        <v>-0.022929936305732503</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.04773101340230422</v>
+        <v>0.013556388808768336</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.05187376725838262</v>
+        <v>-0.06412175648702595</v>
       </c>
     </row>
     <row r="3">
@@ -3127,16 +3127,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>0.025769506084466858</v>
+        <v>0.06816030293467973</v>
       </c>
       <c r="D3" t="n">
-        <v>0.07115531752104057</v>
+        <v>0.0485232067510549</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.03989361702127663</v>
+        <v>0.08266414737836555</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.019656019656019708</v>
+        <v>-0.04821638573108587</v>
       </c>
     </row>
     <row r="4">
@@ -3147,16 +3147,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.016727069974909407</v>
+        <v>0.04176771759633526</v>
       </c>
       <c r="D4" t="n">
-        <v>0.02306248323947438</v>
+        <v>-0.0015455950540958282</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.04545454545454534</v>
+        <v>0.03672612801678912</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.04087385482734326</v>
+        <v>-0.059173357121617524</v>
       </c>
     </row>
     <row r="5">
@@ -3167,16 +3167,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.033558727773603726</v>
+        <v>0.028028028028027997</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0035104142288790107</v>
+        <v>-0.01590348231423095</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.04779233381853468</v>
+        <v>0.01668653158522048</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.04935711323102456</v>
+        <v>-0.06338397066526978</v>
       </c>
     </row>
     <row r="6">
@@ -3187,16 +3187,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.10015649452269182</v>
+        <v>-0.01378070701018572</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.02412380518889394</v>
+        <v>-0.06324110671936757</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.09493670886075943</v>
+        <v>0.010928961748633977</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.12795698924731194</v>
+        <v>-0.14440639269406386</v>
       </c>
     </row>
     <row r="7">
@@ -3207,16 +3207,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.05476107429368675</v>
+        <v>0.00509554140127393</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.009062448508815208</v>
+        <v>-0.02058590657165472</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.05043782837127835</v>
+        <v>0.0071820870299958055</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.05821359798548363</v>
+        <v>-0.06416217221498972</v>
       </c>
     </row>
     <row r="8">
@@ -3227,16 +3227,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.09090909090909088</v>
+        <v>0.0058823529411765035</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0060422960725075164</v>
+        <v>-0.04481132075471696</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.11418685121107258</v>
+        <v>0.018817204301075436</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.13492063492063486</v>
+        <v>-0.1379310344827585</v>
       </c>
     </row>
     <row r="9">
@@ -3247,16 +3247,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.13152173913043486</v>
+        <v>0.0032258064516128837</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.06272000000000003</v>
+        <v>-0.05346350534635058</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.12830735773831095</v>
+        <v>0.005485463521667586</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.14694704839118317</v>
+        <v>-0.13836734693877545</v>
       </c>
     </row>
     <row r="10">
@@ -3267,16 +3267,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.17076923076923076</v>
+        <v>-0.004013220018885693</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.11434591074506806</v>
+        <v>-0.05597897503285147</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.14221652786675207</v>
+        <v>-0.007849293563579284</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.1553690212226797</v>
+        <v>-0.13587715216379712</v>
       </c>
     </row>
     <row r="11">
@@ -3287,16 +3287,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.027893639207507787</v>
+        <v>0.0282478686855834</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.03948080043266631</v>
+        <v>0.026081888387002806</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.06928345626975761</v>
+        <v>0.0017231476163124338</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.04184704184704176</v>
+        <v>0.019201462968607048</v>
       </c>
     </row>
     <row r="12">
@@ -3307,16 +3307,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.04272727272727269</v>
+        <v>-0.05613648871766641</v>
       </c>
       <c r="D12" t="n">
-        <v>0.03519749706687528</v>
+        <v>-0.0762112139357649</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.028864059590316498</v>
+        <v>0.01731879409878114</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.08900687070580877</v>
+        <v>-0.14517625231910955</v>
       </c>
     </row>
     <row r="13">
@@ -3327,16 +3327,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.04873044370351376</v>
+        <v>-0.029202739372011968</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.05791067373202112</v>
+        <v>-0.03418367346938781</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.029418975239029203</v>
+        <v>-0.019283403831798905</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.03518761863045686</v>
+        <v>-0.025254762959680998</v>
       </c>
     </row>
     <row r="14">
@@ -3347,16 +3347,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.1246458923512747</v>
+        <v>-0.29859719438877746</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.13398553806890684</v>
+        <v>-0.18413021363173962</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.05753514220333444</v>
+        <v>-0.08339889850511396</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.056494447126991865</v>
+        <v>-0.1287410926365795</v>
       </c>
     </row>
     <row r="15">
@@ -3367,16 +3367,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>0.16017885323513945</v>
+        <v>0.27280064568200174</v>
       </c>
       <c r="D15" t="n">
-        <v>0.2575849514563106</v>
+        <v>0.34804490902051893</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.01649132783622413</v>
+        <v>0.22982975573649145</v>
       </c>
       <c r="F15" t="n">
-        <v>0.008164275111330948</v>
+        <v>0.1227085671530116</v>
       </c>
     </row>
     <row r="16">
@@ -3387,16 +3387,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.05687652054281785</v>
+        <v>0.02671969863946943</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02891586899845863</v>
+        <v>0.008530350535265227</v>
       </c>
       <c r="E16" t="n">
-        <v>0.04448540074282669</v>
+        <v>0.01378155823002446</v>
       </c>
       <c r="F16" t="n">
-        <v>0.00847077988189786</v>
+        <v>-0.012935748883643993</v>
       </c>
     </row>
     <row r="17">
@@ -3407,16 +3407,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.1778846153846153</v>
+        <v>-0.0815450643776825</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.10294117647058829</v>
+        <v>-0.03389830508474589</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.09090909090909091</v>
+        <v>-0.03984063745019924</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.05263157894736837</v>
+        <v>-0.007462686567164263</v>
       </c>
     </row>
     <row r="18">
@@ -3427,16 +3427,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.038888888888888924</v>
+        <v>0.018231540565177774</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.07075038284839207</v>
+        <v>0.021619927933573608</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.08588252190147935</v>
+        <v>-0.004089669797031257</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.04096889952153107</v>
+        <v>0.029387485553904635</v>
       </c>
     </row>
     <row r="19">
@@ -3447,16 +3447,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.2500000000000001</v>
+        <v>-0.2000000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.47058823529411764</v>
+        <v>0.03846153846153856</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.2857142857142857</v>
+        <v>-0.14285714285714293</v>
       </c>
       <c r="F19" t="n">
-        <v>0.39999999999999997</v>
+        <v>0.8333333333333336</v>
       </c>
     </row>
     <row r="20">
@@ -3467,16 +3467,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.02927019643554062</v>
+        <v>-0.013757861635220065</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.06890720777848239</v>
+        <v>-0.015608521408985483</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.023431294678316044</v>
+        <v>-0.007016596950478994</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.014683975313896492</v>
+        <v>0.026975763962065403</v>
       </c>
     </row>
   </sheetData>
@@ -3518,16 +3518,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.22268907563025206</v>
+        <v>-0.041371158392434895</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1268260292164675</v>
+        <v>-0.003875968992247994</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.057645631067961216</v>
+        <v>-0.04773101340230422</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.28811121764141906</v>
+        <v>-0.05187376725838262</v>
       </c>
     </row>
     <row r="3">
@@ -3538,16 +3538,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.2547085201793723</v>
+        <v>0.025769506084466858</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.10728476821192048</v>
+        <v>0.07115531752104057</v>
       </c>
       <c r="E3" t="n">
-        <v>0.03111111111111108</v>
+        <v>-0.03989361702127663</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.32409739714525604</v>
+        <v>-0.019656019656019708</v>
       </c>
     </row>
     <row r="4">
@@ -3558,16 +3558,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.23458540042523035</v>
+        <v>-0.016727069974909407</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.11830742659758207</v>
+        <v>0.02306248323947438</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.02841781874039945</v>
+        <v>-0.04545454545454534</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.30232558139534876</v>
+        <v>-0.04087385482734326</v>
       </c>
     </row>
     <row r="5">
@@ -3578,16 +3578,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.22539682539682543</v>
+        <v>-0.033558727773603726</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.12243401759530786</v>
+        <v>0.0035104142288790107</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.05296343001261029</v>
+        <v>-0.04779233381853468</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.292197858235594</v>
+        <v>-0.04935711323102456</v>
       </c>
     </row>
     <row r="6">
@@ -3598,16 +3598,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.32423208191126274</v>
+        <v>-0.10015649452269182</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.13513513513513511</v>
+        <v>-0.02412380518889394</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.019543973941368184</v>
+        <v>-0.09493670886075943</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.4437229437229437</v>
+        <v>-0.12795698924731194</v>
       </c>
     </row>
     <row r="7">
@@ -3618,16 +3618,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1961038961038961</v>
+        <v>-0.05476107429368675</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.0957297043641483</v>
+        <v>-0.009062448508815208</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.033949290932531115</v>
+        <v>-0.05043782837127835</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.2613833854709768</v>
+        <v>-0.05821359798548363</v>
       </c>
     </row>
     <row r="8">
@@ -3638,16 +3638,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.3295454545454546</v>
+        <v>-0.09090909090909088</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1447368421052632</v>
+        <v>-0.0060422960725075164</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.044943820224719024</v>
+        <v>-0.11418685121107258</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.4318181818181818</v>
+        <v>-0.13492063492063486</v>
       </c>
     </row>
     <row r="9">
@@ -3658,16 +3658,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.3130841121495327</v>
+        <v>-0.13152173913043486</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.13043478260869562</v>
+        <v>-0.06272000000000003</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.02272727272727275</v>
+        <v>-0.12830735773831095</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.4303405572755418</v>
+        <v>-0.14694704839118317</v>
       </c>
     </row>
     <row r="10">
@@ -3678,16 +3678,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.29255319148936176</v>
+        <v>-0.17076923076923076</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1149068322981366</v>
+        <v>-0.11434591074506806</v>
       </c>
       <c r="E10" t="n">
-        <v>0.006345177664974625</v>
+        <v>-0.14221652786675207</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.4232804232804233</v>
+        <v>-0.1553690212226797</v>
       </c>
     </row>
     <row r="11">
@@ -3698,16 +3698,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.1515723270440252</v>
+        <v>-0.027893639207507787</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.08507386653082014</v>
+        <v>-0.03948080043266631</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.0458874458874458</v>
+        <v>-0.06928345626975761</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.1660377358490565</v>
+        <v>-0.04184704184704176</v>
       </c>
     </row>
     <row r="12">
@@ -3718,16 +3718,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.3485714285714286</v>
+        <v>-0.04272727272727269</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.155223880597015</v>
+        <v>0.03519749706687528</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.018229166666666647</v>
+        <v>-0.028864059590316498</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.4661157024793388</v>
+        <v>-0.08900687070580877</v>
       </c>
     </row>
     <row r="13">
@@ -3738,16 +3738,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.028820210939416193</v>
+        <v>-0.04873044370351376</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.024024390243902367</v>
+        <v>-0.05791067373202112</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.009549461312438686</v>
+        <v>-0.029418975239029203</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.012416979497545395</v>
+        <v>-0.03518761863045686</v>
       </c>
     </row>
     <row r="14">
@@ -3758,16 +3758,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0452240646841168</v>
+        <v>-0.1246458923512747</v>
       </c>
       <c r="D14" t="n">
-        <v>0.03366906474820157</v>
+        <v>-0.13398553806890684</v>
       </c>
       <c r="E14" t="n">
-        <v>0.02627422828427851</v>
+        <v>-0.05753514220333444</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0788629069234296</v>
+        <v>-0.056494447126991865</v>
       </c>
     </row>
     <row r="15">
@@ -3778,16 +3778,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.14483394833948332</v>
+        <v>0.16017885323513945</v>
       </c>
       <c r="D15" t="n">
-        <v>0.10987261146496821</v>
+        <v>0.2575849514563106</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0957642725598526</v>
+        <v>-0.01649132783622413</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.12362204724409454</v>
+        <v>0.008164275111330948</v>
       </c>
     </row>
     <row r="16">
@@ -3798,16 +3798,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.042091301354913374</v>
+        <v>0.05687652054281785</v>
       </c>
       <c r="D16" t="n">
-        <v>0.00973901113178328</v>
+        <v>0.02891586899845863</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.017420116464787687</v>
+        <v>0.04448540074282669</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0016939840673932144</v>
+        <v>0.00847077988189786</v>
       </c>
     </row>
     <row r="17">
@@ -3818,16 +3818,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.09226190476190473</v>
+        <v>-0.1778846153846153</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.0017953321364452938</v>
+        <v>-0.10294117647058829</v>
       </c>
       <c r="E17" t="n">
-        <v>0.1010452961672475</v>
+        <v>-0.09090909090909091</v>
       </c>
       <c r="F17" t="n">
-        <v>0.01257861635220118</v>
+        <v>-0.05263157894736837</v>
       </c>
     </row>
     <row r="18">
@@ -3838,16 +3838,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.15659881812212728</v>
+        <v>-0.038888888888888924</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.09379093528949436</v>
+        <v>-0.07075038284839207</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.03988868274582567</v>
+        <v>-0.08588252190147935</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.15137956748695006</v>
+        <v>-0.04096889952153107</v>
       </c>
     </row>
     <row r="19">
@@ -3858,16 +3858,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.29629629629629634</v>
+        <v>-0.2500000000000001</v>
       </c>
       <c r="D19" t="n">
-        <v>0.233009708737864</v>
+        <v>-0.47058823529411764</v>
       </c>
       <c r="E19" t="n">
-        <v>0.5833333333333335</v>
+        <v>-0.2857142857142857</v>
       </c>
       <c r="F19" t="n">
-        <v>1.3333333333333333</v>
+        <v>0.39999999999999997</v>
       </c>
     </row>
     <row r="20">
@@ -3878,16 +3878,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.013063685466650014</v>
+        <v>-0.02927019643554062</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.0179442508710801</v>
+        <v>-0.06890720777848239</v>
       </c>
       <c r="E20" t="n">
-        <v>0.007094943240454011</v>
+        <v>-0.023431294678316044</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.005648720211826974</v>
+        <v>-0.014683975313896492</v>
       </c>
     </row>
   </sheetData>
@@ -3929,16 +3929,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.12386706948640488</v>
+        <v>-0.22268907563025206</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.09311740890688261</v>
+        <v>-0.1268260292164675</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.11168032786885253</v>
+        <v>-0.057645631067961216</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.11807120324470471</v>
+        <v>-0.28811121764141906</v>
       </c>
     </row>
     <row r="3">
@@ -3949,16 +3949,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.1378839590443686</v>
+        <v>-0.2547085201793723</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.05607476635514011</v>
+        <v>-0.10728476821192048</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.10044642857142856</v>
+        <v>0.03111111111111108</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.11163416274377945</v>
+        <v>-0.32409739714525604</v>
       </c>
     </row>
     <row r="4">
@@ -3969,16 +3969,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.12794033275960995</v>
+        <v>-0.23458540042523035</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.08327501749475154</v>
+        <v>-0.11830742659758207</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.11190903650508674</v>
+        <v>-0.02841781874039945</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.11695906432748535</v>
+        <v>-0.30232558139534876</v>
       </c>
     </row>
     <row r="5">
@@ -3989,16 +3989,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.1229551451187336</v>
+        <v>-0.22539682539682543</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.08785046728971964</v>
+        <v>-0.12243401759530786</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.11152025249868489</v>
+        <v>-0.05296343001261029</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.11856400566839873</v>
+        <v>-0.292197858235594</v>
       </c>
     </row>
     <row r="6">
@@ -4009,16 +4009,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.24791086350974934</v>
+        <v>-0.32423208191126274</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.1409395973154362</v>
+        <v>-0.13513513513513511</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.17971014492753634</v>
+        <v>-0.019543973941368184</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.22601279317697226</v>
+        <v>-0.4437229437229437</v>
       </c>
     </row>
     <row r="7">
@@ -4029,16 +4029,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.120923415170392</v>
+        <v>-0.1961038961038961</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.07603305785123968</v>
+        <v>-0.0957297043641483</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.0945945945945947</v>
+        <v>-0.033949290932531115</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.11331351172778327</v>
+        <v>-0.2613833854709768</v>
       </c>
     </row>
     <row r="8">
@@ -4049,16 +4049,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.2540983606557377</v>
+        <v>-0.3295454545454546</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.11578947368421055</v>
+        <v>-0.1447368421052632</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.17391304347826086</v>
+        <v>-0.044943820224719024</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.2251655629139073</v>
+        <v>-0.4318181818181818</v>
       </c>
     </row>
     <row r="9">
@@ -4069,16 +4069,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.24190800681431013</v>
+        <v>-0.3130841121495327</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.12147505422993493</v>
+        <v>-0.13043478260869562</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.16967509025270755</v>
+        <v>-0.02272727272727275</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.2169680111265647</v>
+        <v>-0.4303405572755418</v>
       </c>
     </row>
     <row r="10">
@@ -4089,16 +4089,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.23205506391347094</v>
+        <v>-0.29255319148936176</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.13135068153655513</v>
+        <v>-0.1149068322981366</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1671891327063741</v>
+        <v>0.006345177664974625</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.20734693877551014</v>
+        <v>-0.4232804232804233</v>
       </c>
     </row>
     <row r="11">
@@ -4109,16 +4109,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.08017334777898148</v>
+        <v>-0.1515723270440252</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.057191634656423365</v>
+        <v>-0.08507386653082014</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.060800790904597155</v>
+        <v>-0.0458874458874458</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0910458991723099</v>
+        <v>-0.1660377358490565</v>
       </c>
     </row>
     <row r="12">
@@ -4129,16 +4129,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.2712933753943218</v>
+        <v>-0.3485714285714286</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.17589576547231275</v>
+        <v>-0.155223880597015</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.20312500000000006</v>
+        <v>-0.018229166666666647</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.2505050505050505</v>
+        <v>-0.4661157024793388</v>
       </c>
     </row>
     <row r="13">
@@ -4149,16 +4149,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.03513022410660209</v>
+        <v>-0.028820210939416193</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.019123020706455465</v>
+        <v>-0.024024390243902367</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.01403808593750008</v>
+        <v>-0.009549461312438686</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.011384925781812808</v>
+        <v>-0.012416979497545395</v>
       </c>
     </row>
     <row r="14">
@@ -4169,16 +4169,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.015508395522388033</v>
+        <v>0.0452240646841168</v>
       </c>
       <c r="D14" t="n">
-        <v>0.020378632581695304</v>
+        <v>0.03366906474820157</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.0017736786094360373</v>
+        <v>0.02627422828427851</v>
       </c>
       <c r="F14" t="n">
-        <v>0.032736177342441004</v>
+        <v>0.0788629069234296</v>
       </c>
     </row>
     <row r="15">
@@ -4189,16 +4189,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.188715953307393</v>
+        <v>-0.14483394833948332</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.10402684563758384</v>
+        <v>0.10987261146496821</v>
       </c>
       <c r="E15" t="n">
-        <v>0.019438444924406006</v>
+        <v>0.0957642725598526</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.13351498637602183</v>
+        <v>-0.12362204724409454</v>
       </c>
     </row>
     <row r="16">
@@ -4209,16 +4209,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>0.07682308232704019</v>
+        <v>0.042091301354913374</v>
       </c>
       <c r="D16" t="n">
-        <v>0.030466301953524833</v>
+        <v>0.00973901113178328</v>
       </c>
       <c r="E16" t="n">
-        <v>0.022615272949535734</v>
+        <v>-0.017420116464787687</v>
       </c>
       <c r="F16" t="n">
-        <v>0.018483885610531072</v>
+        <v>0.0016939840673932144</v>
       </c>
     </row>
     <row r="17">
@@ -4229,16 +4229,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.182089552238806</v>
+        <v>-0.09226190476190473</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.06989247311827958</v>
+        <v>-0.0017953321364452938</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.03952569169960478</v>
+        <v>0.1010452961672475</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.044303797468354486</v>
+        <v>0.01257861635220118</v>
       </c>
     </row>
     <row r="18">
@@ -4249,16 +4249,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.056547619047619097</v>
+        <v>-0.15659881812212728</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.03595812471552125</v>
+        <v>-0.09379093528949436</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.03638368246968023</v>
+        <v>-0.03988868274582567</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.06636060100166943</v>
+        <v>-0.15137956748695006</v>
       </c>
     </row>
     <row r="19">
@@ -4269,16 +4269,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.41379310344827586</v>
+        <v>-0.29629629629629634</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.2000000000000001</v>
+        <v>0.233009708737864</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.11111111111111105</v>
+        <v>0.5833333333333335</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.2222222222222222</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="20">
@@ -4289,16 +4289,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.02832574607991904</v>
+        <v>-0.013063685466650014</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.0482013113592061</v>
+        <v>-0.0179442508710801</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.010800842992623795</v>
+        <v>0.007094943240454011</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.025187566988210078</v>
+        <v>-0.005648720211826974</v>
       </c>
     </row>
   </sheetData>
@@ -4340,16 +4340,16 @@
         <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02087332053742799</v>
+        <v>-0.12386706948640488</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.022929936305732503</v>
+        <v>-0.09311740890688261</v>
       </c>
       <c r="E2" t="n">
-        <v>0.013556388808768336</v>
+        <v>-0.11168032786885253</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.06412175648702595</v>
+        <v>-0.11807120324470471</v>
       </c>
     </row>
     <row r="3">
@@ -4360,16 +4360,16 @@
         <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>0.06816030293467973</v>
+        <v>-0.1378839590443686</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0485232067510549</v>
+        <v>-0.05607476635514011</v>
       </c>
       <c r="E3" t="n">
-        <v>0.08266414737836555</v>
+        <v>-0.10044642857142856</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.04821638573108587</v>
+        <v>-0.11163416274377945</v>
       </c>
     </row>
     <row r="4">
@@ -4380,16 +4380,16 @@
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>0.04176771759633526</v>
+        <v>-0.12794033275960995</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.0015455950540958282</v>
+        <v>-0.08327501749475154</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03672612801678912</v>
+        <v>-0.11190903650508674</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.059173357121617524</v>
+        <v>-0.11695906432748535</v>
       </c>
     </row>
     <row r="5">
@@ -4400,16 +4400,16 @@
         <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>0.028028028028027997</v>
+        <v>-0.1229551451187336</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.01590348231423095</v>
+        <v>-0.08785046728971964</v>
       </c>
       <c r="E5" t="n">
-        <v>0.01668653158522048</v>
+        <v>-0.11152025249868489</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.06338397066526978</v>
+        <v>-0.11856400566839873</v>
       </c>
     </row>
     <row r="6">
@@ -4420,16 +4420,16 @@
         <v>28</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.01378070701018572</v>
+        <v>-0.24791086350974934</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.06324110671936757</v>
+        <v>-0.1409395973154362</v>
       </c>
       <c r="E6" t="n">
-        <v>0.010928961748633977</v>
+        <v>-0.17971014492753634</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.14440639269406386</v>
+        <v>-0.22601279317697226</v>
       </c>
     </row>
     <row r="7">
@@ -4440,16 +4440,16 @@
         <v>29</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00509554140127393</v>
+        <v>-0.120923415170392</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.02058590657165472</v>
+        <v>-0.07603305785123968</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0071820870299958055</v>
+        <v>-0.0945945945945947</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.06416217221498972</v>
+        <v>-0.11331351172778327</v>
       </c>
     </row>
     <row r="8">
@@ -4460,16 +4460,16 @@
         <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.005050505050505078</v>
+        <v>-0.2540983606557377</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.0675675675675675</v>
+        <v>-0.11578947368421055</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.009592326139088671</v>
+        <v>-0.17391304347826086</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.16859504132231407</v>
+        <v>-0.2251655629139073</v>
       </c>
     </row>
     <row r="9">
@@ -4480,16 +4480,16 @@
         <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0032258064516128837</v>
+        <v>-0.24190800681431013</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.05346350534635058</v>
+        <v>-0.12147505422993493</v>
       </c>
       <c r="E9" t="n">
-        <v>0.005485463521667586</v>
+        <v>-0.16967509025270755</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.13836734693877545</v>
+        <v>-0.2169680111265647</v>
       </c>
     </row>
     <row r="10">
@@ -4500,16 +4500,16 @@
         <v>32</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0031914893617020716</v>
+        <v>-0.23205506391347094</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.03899721448467967</v>
+        <v>-0.13135068153655513</v>
       </c>
       <c r="E10" t="n">
-        <v>0.015576323987538955</v>
+        <v>-0.1671891327063741</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.11524774158226123</v>
+        <v>-0.20734693877551014</v>
       </c>
     </row>
     <row r="11">
@@ -4520,16 +4520,16 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0818595250126326</v>
+        <v>-0.08017334777898148</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.06432160804020096</v>
+        <v>-0.057191634656423365</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0032644178454842247</v>
+        <v>-0.060800790904597155</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0788203753351207</v>
+        <v>-0.0910458991723099</v>
       </c>
     </row>
     <row r="12">
@@ -4540,16 +4540,16 @@
         <v>34</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.05613648871766641</v>
+        <v>-0.2712933753943218</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.0762112139357649</v>
+        <v>-0.17589576547231275</v>
       </c>
       <c r="E12" t="n">
-        <v>0.01731879409878114</v>
+        <v>-0.20312500000000006</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.14517625231910955</v>
+        <v>-0.2505050505050505</v>
       </c>
     </row>
     <row r="13">
@@ -4560,16 +4560,16 @@
         <v>35</v>
       </c>
       <c r="C13" t="n">
-        <v>3.2615786040452057E-4</v>
+        <v>-0.03513022410660209</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.006402927052366852</v>
+        <v>-0.019123020706455465</v>
       </c>
       <c r="E13" t="n">
-        <v>9.2571164082391E-4</v>
+        <v>-0.01403808593750008</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.006843800322061183</v>
+        <v>-0.011384925781812808</v>
       </c>
     </row>
     <row r="14">
@@ -4580,16 +4580,16 @@
         <v>36</v>
       </c>
       <c r="C14" t="n">
-        <v>0.03306981405188726</v>
+        <v>-0.015508395522388033</v>
       </c>
       <c r="D14" t="n">
-        <v>0.012870298457783263</v>
+        <v>0.020378632581695304</v>
       </c>
       <c r="E14" t="n">
-        <v>0.011941669537260264</v>
+        <v>-0.0017736786094360373</v>
       </c>
       <c r="F14" t="n">
-        <v>0.03525681674064686</v>
+        <v>0.032736177342441004</v>
       </c>
     </row>
     <row r="15">
@@ -4600,16 +4600,16 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.07627475769068691</v>
+        <v>-0.188715953307393</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.007805724197744996</v>
+        <v>-0.10402684563758384</v>
       </c>
       <c r="E15" t="n">
-        <v>0.17987360233349542</v>
+        <v>0.019438444924406006</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.033112582781456984</v>
+        <v>-0.13351498637602183</v>
       </c>
     </row>
     <row r="16">
@@ -4620,16 +4620,16 @@
         <v>38</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.04716906469126423</v>
+        <v>0.07682308232704019</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.02479854727045745</v>
+        <v>0.030466301953524833</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.05381225797836825</v>
+        <v>0.022615272949535734</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.011869074354466611</v>
+        <v>0.018483885610531072</v>
       </c>
     </row>
     <row r="17">
@@ -4640,16 +4640,16 @@
         <v>39</v>
       </c>
       <c r="C17" t="n">
-        <v>0.041297935103244796</v>
+        <v>-0.182089552238806</v>
       </c>
       <c r="D17" t="n">
-        <v>0.040522875816993535</v>
+        <v>-0.06989247311827958</v>
       </c>
       <c r="E17" t="n">
-        <v>0.11455847255369925</v>
+        <v>-0.03952569169960478</v>
       </c>
       <c r="F17" t="n">
-        <v>0.043902439024390144</v>
+        <v>-0.044303797468354486</v>
       </c>
     </row>
     <row r="18">
@@ -4660,16 +4660,16 @@
         <v>40</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.06781166716020129</v>
+        <v>-0.056547619047619097</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.052389705882352915</v>
+        <v>-0.03595812471552125</v>
       </c>
       <c r="E18" t="n">
-        <v>0.028726708074534157</v>
+        <v>-0.03638368246968023</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.06592039800995024</v>
+        <v>-0.06636060100166943</v>
       </c>
     </row>
     <row r="19">
@@ -4680,16 +4680,16 @@
         <v>41</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.09803921568627459</v>
+        <v>-0.41379310344827586</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6842105263157896</v>
+        <v>-0.2000000000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>0.2173913043478261</v>
+        <v>-0.11111111111111105</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8947368421052632</v>
+        <v>-0.2222222222222222</v>
       </c>
     </row>
     <row r="20">
@@ -4700,16 +4700,16 @@
         <v>42</v>
       </c>
       <c r="C20" t="n">
-        <v>0.011221802358868695</v>
+        <v>-0.02832574607991904</v>
       </c>
       <c r="D20" t="n">
-        <v>0.020729426433915354</v>
+        <v>-0.0482013113592061</v>
       </c>
       <c r="E20" t="n">
-        <v>0.01705426356589145</v>
+        <v>-0.010800842992623795</v>
       </c>
       <c r="F20" t="n">
-        <v>0.01093329107906832</v>
+        <v>-0.025187566988210078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>